<commit_message>
MAJ tableau + lien page accueil
</commit_message>
<xml_diff>
--- a/Tableau_SCRUM_B3D.xlsx
+++ b/Tableau_SCRUM_B3D.xlsx
@@ -822,7 +822,7 @@
       <charset val="1"/>
     </font>
   </fonts>
-  <fills count="8">
+  <fills count="9">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -844,7 +844,7 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFDDDDDD"/>
-        <bgColor rgb="FFCCFFCC"/>
+        <bgColor rgb="FFFCD4D1"/>
       </patternFill>
     </fill>
     <fill>
@@ -857,6 +857,12 @@
       <patternFill patternType="solid">
         <fgColor rgb="FFBA131A"/>
         <bgColor rgb="FFCE181E"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFCD4D1"/>
+        <bgColor rgb="FFDDDDDD"/>
       </patternFill>
     </fill>
     <fill>
@@ -1054,7 +1060,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="87">
+  <cellXfs count="91">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -1239,18 +1245,30 @@
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
+    <xf numFmtId="164" fontId="9" fillId="7" borderId="3" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="9" fillId="7" borderId="3" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
     <xf numFmtId="164" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
+    <xf numFmtId="164" fontId="9" fillId="7" borderId="9" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="9" fillId="0" borderId="3" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
     <xf numFmtId="164" fontId="9" fillId="0" borderId="9" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="9" fillId="0" borderId="3" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
     <xf numFmtId="164" fontId="9" fillId="3" borderId="3" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="left" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -1271,6 +1289,10 @@
       <alignment horizontal="right" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
+    <xf numFmtId="164" fontId="17" fillId="0" borderId="3" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
     <xf numFmtId="164" fontId="19" fillId="2" borderId="6" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -1343,11 +1365,11 @@
       <alignment horizontal="left" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="26" fillId="7" borderId="8" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="26" fillId="8" borderId="8" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="18" fillId="7" borderId="3" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="18" fillId="8" borderId="3" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -1453,7 +1475,7 @@
       <rgbColor rgb="FF99CCFF"/>
       <rgbColor rgb="FFFF99CC"/>
       <rgbColor rgb="FFCC99FF"/>
-      <rgbColor rgb="FFFFCC99"/>
+      <rgbColor rgb="FFFCD4D1"/>
       <rgbColor rgb="FF3366CC"/>
       <rgbColor rgb="FF33CCCC"/>
       <rgbColor rgb="FF99CC00"/>
@@ -1486,10 +1508,10 @@
           <c:layoutTarget val="inner"/>
           <c:xMode val="edge"/>
           <c:yMode val="edge"/>
-          <c:x val="0.134025339642803"/>
-          <c:y val="0.196494088870771"/>
-          <c:w val="0.737215692260724"/>
-          <c:h val="0.672136159804321"/>
+          <c:x val="0.134035569803832"/>
+          <c:y val="0.196514116807665"/>
+          <c:w val="0.737195633921075"/>
+          <c:h val="0.672102741820406"/>
         </c:manualLayout>
       </c:layout>
       <c:lineChart>
@@ -1851,11 +1873,11 @@
           </c:spPr>
         </c:hiLowLines>
         <c:marker val="1"/>
-        <c:axId val="32717434"/>
-        <c:axId val="52970127"/>
+        <c:axId val="70068314"/>
+        <c:axId val="6673470"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="32717434"/>
+        <c:axId val="70068314"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1903,14 +1925,14 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="52970127"/>
+        <c:crossAx val="6673470"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="52970127"/>
+        <c:axId val="6673470"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1954,7 +1976,7 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="32717434"/>
+        <c:crossAx val="70068314"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -2211,11 +2233,11 @@
           </c:spPr>
         </c:hiLowLines>
         <c:marker val="1"/>
-        <c:axId val="63565614"/>
-        <c:axId val="29153844"/>
+        <c:axId val="7754835"/>
+        <c:axId val="54543078"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="63565614"/>
+        <c:axId val="7754835"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2241,14 +2263,14 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="29153844"/>
+        <c:crossAx val="54543078"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="29153844"/>
+        <c:axId val="54543078"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2283,7 +2305,7 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="63565614"/>
+        <c:crossAx val="7754835"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -2530,11 +2552,11 @@
           </c:spPr>
         </c:hiLowLines>
         <c:marker val="1"/>
-        <c:axId val="88998366"/>
-        <c:axId val="12017959"/>
+        <c:axId val="30328266"/>
+        <c:axId val="53304297"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="88998366"/>
+        <c:axId val="30328266"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2560,14 +2582,14 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="12017959"/>
+        <c:crossAx val="53304297"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="12017959"/>
+        <c:axId val="53304297"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2602,7 +2624,7 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="88998366"/>
+        <c:crossAx val="30328266"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -2849,11 +2871,11 @@
           </c:spPr>
         </c:hiLowLines>
         <c:marker val="1"/>
-        <c:axId val="17407024"/>
-        <c:axId val="76729517"/>
+        <c:axId val="67935151"/>
+        <c:axId val="99656486"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="17407024"/>
+        <c:axId val="67935151"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2879,14 +2901,14 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="76729517"/>
+        <c:crossAx val="99656486"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="76729517"/>
+        <c:axId val="99656486"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2921,7 +2943,7 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="17407024"/>
+        <c:crossAx val="67935151"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -2976,9 +2998,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>5</xdr:col>
-      <xdr:colOff>915480</xdr:colOff>
+      <xdr:colOff>915120</xdr:colOff>
       <xdr:row>20</xdr:row>
-      <xdr:rowOff>205560</xdr:rowOff>
+      <xdr:rowOff>205200</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame>
       <xdr:nvGraphicFramePr>
@@ -2987,7 +3009,7 @@
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
         <a:off x="1718280" y="3404520"/>
-        <a:ext cx="4716360" cy="3531960"/>
+        <a:ext cx="4716000" cy="3531600"/>
       </xdr:xfrm>
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
@@ -3011,9 +3033,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>12</xdr:col>
-      <xdr:colOff>76680</xdr:colOff>
+      <xdr:colOff>76320</xdr:colOff>
       <xdr:row>22</xdr:row>
-      <xdr:rowOff>297720</xdr:rowOff>
+      <xdr:rowOff>297360</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame>
       <xdr:nvGraphicFramePr>
@@ -3022,7 +3044,7 @@
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
         <a:off x="13459680" y="1436040"/>
-        <a:ext cx="4093920" cy="5616000"/>
+        <a:ext cx="4093560" cy="5615640"/>
       </xdr:xfrm>
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
@@ -3046,9 +3068,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>12</xdr:col>
-      <xdr:colOff>77400</xdr:colOff>
+      <xdr:colOff>77040</xdr:colOff>
       <xdr:row>17</xdr:row>
-      <xdr:rowOff>109080</xdr:rowOff>
+      <xdr:rowOff>108720</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame>
       <xdr:nvGraphicFramePr>
@@ -3057,7 +3079,7 @@
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
         <a:off x="13459680" y="1436040"/>
-        <a:ext cx="4094640" cy="3318480"/>
+        <a:ext cx="4094280" cy="3318120"/>
       </xdr:xfrm>
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
@@ -3081,9 +3103,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>12</xdr:col>
-      <xdr:colOff>76320</xdr:colOff>
+      <xdr:colOff>75960</xdr:colOff>
       <xdr:row>17</xdr:row>
-      <xdr:rowOff>186480</xdr:rowOff>
+      <xdr:rowOff>186120</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame>
       <xdr:nvGraphicFramePr>
@@ -3092,7 +3114,7 @@
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
         <a:off x="13459680" y="1436040"/>
-        <a:ext cx="4093560" cy="3395880"/>
+        <a:ext cx="4093200" cy="3395520"/>
       </xdr:xfrm>
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
@@ -3112,7 +3134,7 @@
   </sheetPr>
   <dimension ref="A1:AMJ1048576"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="65" zoomScaleNormal="65" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="75" zoomScaleNormal="75" zoomScalePageLayoutView="100" workbookViewId="0">
       <pane xSplit="0" ySplit="7" topLeftCell="A8" activePane="bottomLeft" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
       <selection pane="bottomLeft" activeCell="L17" activeCellId="0" sqref="L17"/>
@@ -4465,10 +4487,10 @@
   </sheetPr>
   <dimension ref="A1:AMJ52"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="C1" colorId="64" zoomScale="65" zoomScaleNormal="65" zoomScalePageLayoutView="100" workbookViewId="0">
-      <pane xSplit="0" ySplit="9" topLeftCell="D25" activePane="bottomLeft" state="frozen"/>
-      <selection pane="topLeft" activeCell="C1" activeCellId="0" sqref="C1"/>
-      <selection pane="bottomLeft" activeCell="D14" activeCellId="0" sqref="D14"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="75" zoomScaleNormal="75" zoomScalePageLayoutView="100" workbookViewId="0">
+      <pane xSplit="0" ySplit="9" topLeftCell="D19" activePane="bottomLeft" state="frozen"/>
+      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
+      <selection pane="bottomLeft" activeCell="F25" activeCellId="0" sqref="F25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -4685,76 +4707,76 @@
     <row r="13" customFormat="false" ht="26.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A13" s="42"/>
       <c r="B13" s="42"/>
-      <c r="C13" s="44" t="s">
+      <c r="C13" s="46" t="s">
         <v>64</v>
       </c>
-      <c r="D13" s="45" t="n">
+      <c r="D13" s="47" t="n">
         <v>6</v>
       </c>
-      <c r="E13" s="45" t="n">
+      <c r="E13" s="47" t="n">
         <v>0</v>
       </c>
-      <c r="F13" s="45" t="n">
+      <c r="F13" s="47" t="n">
         <v>0</v>
       </c>
-      <c r="G13" s="45"/>
-      <c r="H13" s="45"/>
+      <c r="G13" s="47"/>
+      <c r="H13" s="47"/>
     </row>
     <row r="14" customFormat="false" ht="26.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A14" s="42"/>
       <c r="B14" s="43"/>
-      <c r="C14" s="44" t="s">
+      <c r="C14" s="46" t="s">
         <v>65</v>
       </c>
-      <c r="D14" s="45" t="n">
+      <c r="D14" s="47" t="n">
         <v>2</v>
       </c>
-      <c r="E14" s="45" t="n">
+      <c r="E14" s="47" t="n">
         <v>2</v>
       </c>
-      <c r="F14" s="45" t="n">
+      <c r="F14" s="47" t="n">
         <v>0</v>
       </c>
-      <c r="G14" s="45"/>
-      <c r="H14" s="45"/>
+      <c r="G14" s="47"/>
+      <c r="H14" s="47"/>
     </row>
     <row r="15" customFormat="false" ht="26.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A15" s="42"/>
       <c r="B15" s="42"/>
-      <c r="C15" s="44" t="s">
+      <c r="C15" s="46" t="s">
         <v>66</v>
       </c>
-      <c r="D15" s="45" t="n">
+      <c r="D15" s="47" t="n">
         <v>2</v>
       </c>
-      <c r="E15" s="45" t="n">
+      <c r="E15" s="47" t="n">
         <v>0</v>
       </c>
-      <c r="F15" s="45" t="n">
+      <c r="F15" s="47" t="n">
         <v>0</v>
       </c>
-      <c r="G15" s="45"/>
-      <c r="H15" s="45"/>
+      <c r="G15" s="47"/>
+      <c r="H15" s="47"/>
     </row>
     <row r="16" customFormat="false" ht="26.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A16" s="42"/>
       <c r="B16" s="42"/>
-      <c r="C16" s="44" t="s">
+      <c r="C16" s="46" t="s">
         <v>67</v>
       </c>
-      <c r="D16" s="45" t="n">
+      <c r="D16" s="47" t="n">
         <v>12</v>
       </c>
-      <c r="E16" s="45" t="n">
+      <c r="E16" s="47" t="n">
         <v>6</v>
       </c>
-      <c r="F16" s="45" t="n">
+      <c r="F16" s="47" t="n">
         <v>0</v>
       </c>
-      <c r="G16" s="45"/>
-      <c r="H16" s="45"/>
-      <c r="I16" s="46"/>
-      <c r="J16" s="46"/>
+      <c r="G16" s="47"/>
+      <c r="H16" s="47"/>
+      <c r="I16" s="48"/>
+      <c r="J16" s="48"/>
     </row>
     <row r="17" customFormat="false" ht="26.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A17" s="42"/>
@@ -4777,25 +4799,25 @@
     <row r="18" customFormat="false" ht="26.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A18" s="42"/>
       <c r="B18" s="42"/>
-      <c r="C18" s="47" t="s">
+      <c r="C18" s="49" t="s">
         <v>69</v>
       </c>
-      <c r="D18" s="45" t="n">
+      <c r="D18" s="47" t="n">
         <v>1</v>
       </c>
-      <c r="E18" s="45" t="n">
+      <c r="E18" s="47" t="n">
         <v>1</v>
       </c>
-      <c r="F18" s="45" t="n">
+      <c r="F18" s="47" t="n">
         <v>0</v>
       </c>
-      <c r="G18" s="45"/>
-      <c r="H18" s="45"/>
+      <c r="G18" s="47"/>
+      <c r="H18" s="47"/>
     </row>
     <row r="19" customFormat="false" ht="26.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A19" s="42"/>
       <c r="B19" s="42"/>
-      <c r="C19" s="48" t="s">
+      <c r="C19" s="50" t="s">
         <v>70</v>
       </c>
       <c r="D19" s="45" t="n">
@@ -4817,20 +4839,20 @@
       <c r="B20" s="43" t="s">
         <v>72</v>
       </c>
-      <c r="C20" s="47" t="s">
+      <c r="C20" s="49" t="s">
         <v>73</v>
       </c>
-      <c r="D20" s="45" t="n">
+      <c r="D20" s="47" t="n">
         <v>4</v>
       </c>
-      <c r="E20" s="45" t="n">
+      <c r="E20" s="47" t="n">
         <v>0</v>
       </c>
-      <c r="F20" s="45" t="n">
+      <c r="F20" s="47" t="n">
         <v>0</v>
       </c>
-      <c r="G20" s="45"/>
-      <c r="H20" s="45"/>
+      <c r="G20" s="47"/>
+      <c r="H20" s="47"/>
     </row>
     <row r="21" customFormat="false" ht="26.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A21" s="42" t="s">
@@ -4839,7 +4861,7 @@
       <c r="B21" s="43" t="s">
         <v>72</v>
       </c>
-      <c r="C21" s="47" t="s">
+      <c r="C21" s="51" t="s">
         <v>74</v>
       </c>
       <c r="D21" s="45" t="n">
@@ -4861,7 +4883,7 @@
       <c r="B22" s="43" t="s">
         <v>72</v>
       </c>
-      <c r="C22" s="47" t="s">
+      <c r="C22" s="51" t="s">
         <v>75</v>
       </c>
       <c r="D22" s="45" t="n">
@@ -4879,10 +4901,10 @@
     <row r="23" customFormat="false" ht="26.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A23" s="42"/>
       <c r="B23" s="42"/>
-      <c r="C23" s="49" t="s">
+      <c r="C23" s="52" t="s">
         <v>76</v>
       </c>
-      <c r="D23" s="50" t="n">
+      <c r="D23" s="53" t="n">
         <v>1</v>
       </c>
       <c r="E23" s="45" t="n">
@@ -4893,60 +4915,60 @@
       </c>
       <c r="G23" s="45"/>
       <c r="H23" s="45"/>
-      <c r="I23" s="46"/>
-      <c r="J23" s="46"/>
+      <c r="I23" s="48"/>
+      <c r="J23" s="48"/>
     </row>
     <row r="24" customFormat="false" ht="27.65" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A24" s="42"/>
-      <c r="B24" s="51" t="s">
+      <c r="B24" s="54" t="s">
         <v>77</v>
       </c>
-      <c r="C24" s="51"/>
-      <c r="D24" s="51"/>
-      <c r="E24" s="51"/>
-      <c r="F24" s="51"/>
-      <c r="G24" s="51"/>
-      <c r="H24" s="51"/>
+      <c r="C24" s="54"/>
+      <c r="D24" s="54"/>
+      <c r="E24" s="54"/>
+      <c r="F24" s="54"/>
+      <c r="G24" s="54"/>
+      <c r="H24" s="54"/>
     </row>
     <row r="25" customFormat="false" ht="27.65" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A25" s="42"/>
-      <c r="B25" s="52" t="s">
+      <c r="B25" s="55" t="s">
         <v>78</v>
       </c>
-      <c r="C25" s="53" t="n">
+      <c r="C25" s="56" t="n">
         <f aca="false">SUM(D11:D24)</f>
         <v>62</v>
       </c>
-      <c r="D25" s="52" t="n">
+      <c r="D25" s="57" t="n">
         <f aca="false">SUM(D11:D23)</f>
         <v>62</v>
       </c>
-      <c r="E25" s="45" t="n">
+      <c r="E25" s="57" t="n">
         <f aca="false">SUM(E11:E23)</f>
         <v>37</v>
       </c>
-      <c r="F25" s="45" t="n">
+      <c r="F25" s="57" t="n">
         <f aca="false">SUM(F14:F23)</f>
         <v>17</v>
       </c>
-      <c r="G25" s="45" t="n">
+      <c r="G25" s="57" t="n">
         <f aca="false">SUM(G14:G23)</f>
         <v>0</v>
       </c>
-      <c r="H25" s="45" t="n">
+      <c r="H25" s="57" t="n">
         <f aca="false">SUM(H14:H23)</f>
         <v>0</v>
       </c>
     </row>
     <row r="26" customFormat="false" ht="11.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A26" s="54"/>
-      <c r="B26" s="55"/>
-      <c r="C26" s="56"/>
-      <c r="D26" s="55"/>
-      <c r="E26" s="57"/>
-      <c r="F26" s="57"/>
-      <c r="G26" s="57"/>
-      <c r="H26" s="57"/>
+      <c r="A26" s="58"/>
+      <c r="B26" s="59"/>
+      <c r="C26" s="60"/>
+      <c r="D26" s="59"/>
+      <c r="E26" s="61"/>
+      <c r="F26" s="61"/>
+      <c r="G26" s="61"/>
+      <c r="H26" s="61"/>
     </row>
     <row r="27" customFormat="false" ht="24.2" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A27" s="42" t="s">
@@ -5019,7 +5041,7 @@
       <c r="B31" s="43" t="s">
         <v>72</v>
       </c>
-      <c r="C31" s="47" t="s">
+      <c r="C31" s="51" t="s">
         <v>82</v>
       </c>
       <c r="D31" s="45" t="n">
@@ -5047,7 +5069,7 @@
     <row r="33" customFormat="false" ht="24.2" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A33" s="42"/>
       <c r="B33" s="42"/>
-      <c r="C33" s="48" t="s">
+      <c r="C33" s="50" t="s">
         <v>83</v>
       </c>
       <c r="D33" s="45" t="n">
@@ -5057,13 +5079,13 @@
       <c r="F33" s="45"/>
       <c r="G33" s="45"/>
       <c r="H33" s="45"/>
-      <c r="I33" s="46"/>
-      <c r="J33" s="46"/>
+      <c r="I33" s="48"/>
+      <c r="J33" s="48"/>
     </row>
     <row r="34" customFormat="false" ht="24.2" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A34" s="42"/>
       <c r="B34" s="42"/>
-      <c r="C34" s="47" t="s">
+      <c r="C34" s="51" t="s">
         <v>84</v>
       </c>
       <c r="D34" s="45" t="n">
@@ -5077,7 +5099,7 @@
     <row r="35" customFormat="false" ht="24.2" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A35" s="42"/>
       <c r="B35" s="42"/>
-      <c r="C35" s="48" t="s">
+      <c r="C35" s="50" t="s">
         <v>85</v>
       </c>
       <c r="D35" s="45" t="n">
@@ -5091,10 +5113,10 @@
     <row r="36" customFormat="false" ht="24.2" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A36" s="42"/>
       <c r="B36" s="42"/>
-      <c r="C36" s="49" t="s">
+      <c r="C36" s="52" t="s">
         <v>76</v>
       </c>
-      <c r="D36" s="50" t="n">
+      <c r="D36" s="53" t="n">
         <v>1</v>
       </c>
       <c r="E36" s="45"/>
@@ -5104,42 +5126,42 @@
     </row>
     <row r="37" customFormat="false" ht="24.2" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A37" s="42"/>
-      <c r="B37" s="51" t="s">
+      <c r="B37" s="54" t="s">
         <v>77</v>
       </c>
-      <c r="C37" s="51"/>
-      <c r="D37" s="51"/>
-      <c r="E37" s="58"/>
-      <c r="F37" s="58"/>
-      <c r="G37" s="58"/>
-      <c r="H37" s="58"/>
+      <c r="C37" s="54"/>
+      <c r="D37" s="54"/>
+      <c r="E37" s="62"/>
+      <c r="F37" s="62"/>
+      <c r="G37" s="62"/>
+      <c r="H37" s="62"/>
     </row>
     <row r="38" customFormat="false" ht="24.2" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A38" s="42"/>
-      <c r="B38" s="52" t="s">
+      <c r="B38" s="55" t="s">
         <v>78</v>
       </c>
-      <c r="C38" s="53" t="n">
+      <c r="C38" s="56" t="n">
         <f aca="false">SUM(D27:D37)</f>
         <v>39</v>
       </c>
-      <c r="D38" s="52"/>
-      <c r="E38" s="59"/>
-      <c r="F38" s="59"/>
-      <c r="G38" s="59"/>
-      <c r="H38" s="59"/>
+      <c r="D38" s="55"/>
+      <c r="E38" s="63"/>
+      <c r="F38" s="63"/>
+      <c r="G38" s="63"/>
+      <c r="H38" s="63"/>
       <c r="I38" s="32"/>
       <c r="J38" s="32"/>
     </row>
     <row r="39" customFormat="false" ht="11.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A39" s="54"/>
-      <c r="B39" s="55"/>
-      <c r="C39" s="56"/>
-      <c r="D39" s="55"/>
-      <c r="E39" s="57"/>
-      <c r="F39" s="57"/>
-      <c r="G39" s="57"/>
-      <c r="H39" s="57"/>
+      <c r="A39" s="58"/>
+      <c r="B39" s="59"/>
+      <c r="C39" s="60"/>
+      <c r="D39" s="59"/>
+      <c r="E39" s="61"/>
+      <c r="F39" s="61"/>
+      <c r="G39" s="61"/>
+      <c r="H39" s="61"/>
     </row>
     <row r="40" customFormat="false" ht="25.35" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A40" s="42" t="s">
@@ -5212,7 +5234,7 @@
       <c r="B44" s="43" t="s">
         <v>72</v>
       </c>
-      <c r="C44" s="47" t="s">
+      <c r="C44" s="51" t="s">
         <v>82</v>
       </c>
       <c r="D44" s="45" t="n">
@@ -5240,7 +5262,7 @@
     <row r="46" customFormat="false" ht="25.35" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A46" s="42"/>
       <c r="B46" s="42"/>
-      <c r="C46" s="48" t="s">
+      <c r="C46" s="50" t="s">
         <v>83</v>
       </c>
       <c r="D46" s="45" t="n">
@@ -5254,7 +5276,7 @@
     <row r="47" customFormat="false" ht="25.35" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A47" s="42"/>
       <c r="B47" s="42"/>
-      <c r="C47" s="47" t="s">
+      <c r="C47" s="51" t="s">
         <v>84</v>
       </c>
       <c r="D47" s="45" t="n">
@@ -5268,7 +5290,7 @@
     <row r="48" customFormat="false" ht="25.35" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A48" s="42"/>
       <c r="B48" s="42"/>
-      <c r="C48" s="48" t="s">
+      <c r="C48" s="50" t="s">
         <v>85</v>
       </c>
       <c r="D48" s="45" t="n">
@@ -5282,10 +5304,10 @@
     <row r="49" customFormat="false" ht="25.35" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A49" s="42"/>
       <c r="B49" s="42"/>
-      <c r="C49" s="49" t="s">
+      <c r="C49" s="52" t="s">
         <v>76</v>
       </c>
-      <c r="D49" s="50" t="n">
+      <c r="D49" s="53" t="n">
         <v>1</v>
       </c>
       <c r="E49" s="45"/>
@@ -5295,40 +5317,40 @@
     </row>
     <row r="50" customFormat="false" ht="25.35" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A50" s="42"/>
-      <c r="B50" s="51" t="s">
+      <c r="B50" s="54" t="s">
         <v>77</v>
       </c>
-      <c r="C50" s="51"/>
-      <c r="D50" s="51"/>
-      <c r="E50" s="51"/>
-      <c r="F50" s="51"/>
-      <c r="G50" s="51"/>
-      <c r="H50" s="51"/>
+      <c r="C50" s="54"/>
+      <c r="D50" s="54"/>
+      <c r="E50" s="54"/>
+      <c r="F50" s="54"/>
+      <c r="G50" s="54"/>
+      <c r="H50" s="54"/>
     </row>
     <row r="51" customFormat="false" ht="25.35" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A51" s="42"/>
-      <c r="B51" s="52" t="s">
+      <c r="B51" s="55" t="s">
         <v>78</v>
       </c>
-      <c r="C51" s="53" t="n">
+      <c r="C51" s="56" t="n">
         <f aca="false">SUM(D40:D50)</f>
         <v>39</v>
       </c>
-      <c r="D51" s="52"/>
-      <c r="E51" s="52"/>
-      <c r="F51" s="52"/>
-      <c r="G51" s="52"/>
-      <c r="H51" s="52"/>
+      <c r="D51" s="55"/>
+      <c r="E51" s="55"/>
+      <c r="F51" s="55"/>
+      <c r="G51" s="55"/>
+      <c r="H51" s="55"/>
     </row>
     <row r="52" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A52" s="60"/>
-      <c r="B52" s="61"/>
-      <c r="C52" s="62"/>
-      <c r="D52" s="63"/>
-      <c r="E52" s="63"/>
-      <c r="F52" s="63"/>
-      <c r="G52" s="63"/>
-      <c r="H52" s="64"/>
+      <c r="A52" s="64"/>
+      <c r="B52" s="65"/>
+      <c r="C52" s="66"/>
+      <c r="D52" s="67"/>
+      <c r="E52" s="67"/>
+      <c r="F52" s="67"/>
+      <c r="G52" s="67"/>
+      <c r="H52" s="68"/>
     </row>
   </sheetData>
   <mergeCells count="10">
@@ -5360,105 +5382,105 @@
   </sheetPr>
   <dimension ref="A1:F10"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="65" zoomScaleNormal="65" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="75" zoomScaleNormal="75" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="I11" activeCellId="0" sqref="I11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="65" width="23.51"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="2" style="65" width="13.68"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="69" width="23.51"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="2" style="69" width="13.68"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="18" min="7" style="0" width="13.68"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="19" style="65" width="14.43"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="19" style="69" width="14.43"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="26.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A1" s="66"/>
-      <c r="B1" s="67"/>
-      <c r="C1" s="68"/>
-      <c r="D1" s="68"/>
-      <c r="E1" s="68"/>
-      <c r="F1" s="69" t="s">
+      <c r="A1" s="70"/>
+      <c r="B1" s="71"/>
+      <c r="C1" s="72"/>
+      <c r="D1" s="72"/>
+      <c r="E1" s="72"/>
+      <c r="F1" s="73" t="s">
         <v>87</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="26.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B2" s="67"/>
-      <c r="C2" s="68"/>
-      <c r="D2" s="68"/>
-      <c r="E2" s="68"/>
-      <c r="F2" s="70"/>
+      <c r="B2" s="71"/>
+      <c r="C2" s="72"/>
+      <c r="D2" s="72"/>
+      <c r="E2" s="72"/>
+      <c r="F2" s="74"/>
     </row>
     <row r="3" customFormat="false" ht="26.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B3" s="67"/>
-      <c r="C3" s="68"/>
-      <c r="D3" s="68"/>
-      <c r="E3" s="68"/>
-      <c r="F3" s="70"/>
+      <c r="B3" s="71"/>
+      <c r="C3" s="72"/>
+      <c r="D3" s="72"/>
+      <c r="E3" s="72"/>
+      <c r="F3" s="74"/>
     </row>
     <row r="4" customFormat="false" ht="26.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B4" s="67"/>
-      <c r="C4" s="71"/>
-      <c r="D4" s="68"/>
-      <c r="E4" s="68"/>
-      <c r="F4" s="70"/>
+      <c r="B4" s="71"/>
+      <c r="C4" s="75"/>
+      <c r="D4" s="72"/>
+      <c r="E4" s="72"/>
+      <c r="F4" s="74"/>
     </row>
     <row r="5" customFormat="false" ht="26.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
     <row r="6" customFormat="false" ht="26.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
     <row r="7" customFormat="false" ht="26.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A7" s="72" t="s">
+      <c r="A7" s="76" t="s">
         <v>54</v>
       </c>
-      <c r="B7" s="73" t="s">
+      <c r="B7" s="77" t="s">
         <v>55</v>
       </c>
-      <c r="C7" s="73" t="s">
+      <c r="C7" s="77" t="s">
         <v>88</v>
       </c>
-      <c r="D7" s="73" t="s">
+      <c r="D7" s="77" t="s">
         <v>89</v>
       </c>
-      <c r="E7" s="73" t="s">
+      <c r="E7" s="77" t="s">
         <v>90</v>
       </c>
-      <c r="F7" s="73" t="s">
+      <c r="F7" s="77" t="s">
         <v>91</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="26.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A8" s="72" t="s">
+      <c r="A8" s="76" t="s">
         <v>58</v>
       </c>
-      <c r="B8" s="74" t="n">
+      <c r="B8" s="78" t="n">
         <f aca="false">SUM(B10:B18,B22:B23)</f>
         <v>0</v>
       </c>
-      <c r="C8" s="74" t="n">
+      <c r="C8" s="78" t="n">
         <f aca="false">SUM(C10:C18)</f>
         <v>0</v>
       </c>
-      <c r="D8" s="74" t="n">
+      <c r="D8" s="78" t="n">
         <f aca="false">SUM(D10:D18)</f>
         <v>0</v>
       </c>
-      <c r="E8" s="74" t="n">
+      <c r="E8" s="78" t="n">
         <f aca="false">SUM(E10:E18)</f>
         <v>0</v>
       </c>
-      <c r="F8" s="74" t="n">
+      <c r="F8" s="78" t="n">
         <f aca="false">SUM(F10:F18)</f>
         <v>0</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="26.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A9" s="72" t="s">
+      <c r="A9" s="76" t="s">
         <v>59</v>
       </c>
-      <c r="B9" s="74"/>
-      <c r="C9" s="74"/>
-      <c r="D9" s="74"/>
-      <c r="E9" s="74"/>
-      <c r="F9" s="74" t="e">
+      <c r="B9" s="78"/>
+      <c r="C9" s="78"/>
+      <c r="D9" s="78"/>
+      <c r="E9" s="78"/>
+      <c r="F9" s="78" t="e">
         <f aca="false">SUM(#REF!)</f>
         <v>#REF!</v>
       </c>
@@ -5501,7 +5523,7 @@
   </sheetPr>
   <dimension ref="A1:AMJ25"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A4" colorId="64" zoomScale="65" zoomScaleNormal="65" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A4" colorId="64" zoomScale="75" zoomScaleNormal="75" zoomScalePageLayoutView="100" workbookViewId="0">
       <pane xSplit="3" ySplit="0" topLeftCell="D4" activePane="topRight" state="frozen"/>
       <selection pane="topLeft" activeCell="A4" activeCellId="0" sqref="A4"/>
       <selection pane="topRight" activeCell="A11" activeCellId="0" sqref="A11"/>
@@ -5600,11 +5622,11 @@
       <c r="F7" s="37"/>
       <c r="G7" s="37"/>
       <c r="H7" s="37"/>
-      <c r="I7" s="75"/>
-      <c r="Q7" s="76"/>
-      <c r="R7" s="77"/>
-      <c r="S7" s="77"/>
-      <c r="T7" s="78"/>
+      <c r="I7" s="79"/>
+      <c r="Q7" s="80"/>
+      <c r="R7" s="81"/>
+      <c r="S7" s="81"/>
+      <c r="T7" s="82"/>
     </row>
     <row r="8" customFormat="false" ht="20.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A8" s="36"/>
@@ -5627,10 +5649,10 @@
       <c r="H8" s="40" t="s">
         <v>91</v>
       </c>
-      <c r="Q8" s="76"/>
-      <c r="R8" s="77"/>
-      <c r="S8" s="77"/>
-      <c r="T8" s="79"/>
+      <c r="Q8" s="80"/>
+      <c r="R8" s="81"/>
+      <c r="S8" s="81"/>
+      <c r="T8" s="83"/>
     </row>
     <row r="9" customFormat="false" ht="20.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A9" s="36"/>
@@ -5658,8 +5680,8 @@
         <f aca="false">SUM(H11:H24)</f>
         <v>0</v>
       </c>
-      <c r="Q9" s="80"/>
-      <c r="T9" s="79"/>
+      <c r="Q9" s="84"/>
+      <c r="T9" s="83"/>
     </row>
     <row r="10" customFormat="false" ht="20.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A10" s="36"/>
@@ -5675,14 +5697,14 @@
         <f aca="false">SUM(#REF!)</f>
         <v>#REF!</v>
       </c>
-      <c r="Q10" s="80"/>
-      <c r="T10" s="79"/>
+      <c r="Q10" s="84"/>
+      <c r="T10" s="83"/>
     </row>
     <row r="11" s="1" customFormat="true" ht="27.65" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A11" s="42" t="s">
         <v>60</v>
       </c>
-      <c r="B11" s="81" t="s">
+      <c r="B11" s="85" t="s">
         <v>92</v>
       </c>
       <c r="C11" s="44" t="s">
@@ -5697,8 +5719,8 @@
       <c r="F11" s="45"/>
       <c r="G11" s="45"/>
       <c r="H11" s="45"/>
-      <c r="Q11" s="82"/>
-      <c r="T11" s="83"/>
+      <c r="Q11" s="86"/>
+      <c r="T11" s="87"/>
       <c r="AMF11" s="0"/>
       <c r="AMG11" s="0"/>
       <c r="AMH11" s="0"/>
@@ -5720,8 +5742,8 @@
       <c r="F12" s="45"/>
       <c r="G12" s="45"/>
       <c r="H12" s="45"/>
-      <c r="Q12" s="82"/>
-      <c r="T12" s="83"/>
+      <c r="Q12" s="86"/>
+      <c r="T12" s="87"/>
       <c r="AMF12" s="0"/>
       <c r="AMG12" s="0"/>
       <c r="AMH12" s="0"/>
@@ -5743,8 +5765,8 @@
       <c r="F13" s="45"/>
       <c r="G13" s="45"/>
       <c r="H13" s="45"/>
-      <c r="Q13" s="82"/>
-      <c r="T13" s="83"/>
+      <c r="Q13" s="86"/>
+      <c r="T13" s="87"/>
       <c r="AMF13" s="0"/>
       <c r="AMG13" s="0"/>
       <c r="AMH13" s="0"/>
@@ -5753,7 +5775,7 @@
     </row>
     <row r="14" s="1" customFormat="true" ht="27.65" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A14" s="42"/>
-      <c r="B14" s="81"/>
+      <c r="B14" s="85"/>
       <c r="C14" s="44" t="s">
         <v>65</v>
       </c>
@@ -5764,8 +5786,8 @@
       <c r="F14" s="45"/>
       <c r="G14" s="45"/>
       <c r="H14" s="45"/>
-      <c r="Q14" s="82"/>
-      <c r="T14" s="83"/>
+      <c r="Q14" s="86"/>
+      <c r="T14" s="87"/>
       <c r="AMF14" s="0"/>
       <c r="AMG14" s="0"/>
       <c r="AMH14" s="0"/>
@@ -5785,8 +5807,8 @@
       <c r="F15" s="45"/>
       <c r="G15" s="45"/>
       <c r="H15" s="45"/>
-      <c r="Q15" s="82"/>
-      <c r="T15" s="83"/>
+      <c r="Q15" s="86"/>
+      <c r="T15" s="87"/>
       <c r="AMF15" s="0"/>
       <c r="AMG15" s="0"/>
       <c r="AMH15" s="0"/>
@@ -5806,8 +5828,8 @@
       <c r="F16" s="45"/>
       <c r="G16" s="45"/>
       <c r="H16" s="45"/>
-      <c r="Q16" s="82"/>
-      <c r="T16" s="83"/>
+      <c r="Q16" s="86"/>
+      <c r="T16" s="87"/>
       <c r="AMF16" s="0"/>
       <c r="AMG16" s="0"/>
       <c r="AMH16" s="0"/>
@@ -5818,10 +5840,10 @@
       <c r="A17" s="42" t="s">
         <v>71</v>
       </c>
-      <c r="B17" s="81" t="s">
+      <c r="B17" s="85" t="s">
         <v>72</v>
       </c>
-      <c r="C17" s="47" t="s">
+      <c r="C17" s="51" t="s">
         <v>82</v>
       </c>
       <c r="D17" s="45" t="n">
@@ -5831,8 +5853,8 @@
       <c r="F17" s="45"/>
       <c r="G17" s="45"/>
       <c r="H17" s="45"/>
-      <c r="Q17" s="82"/>
-      <c r="T17" s="83"/>
+      <c r="Q17" s="86"/>
+      <c r="T17" s="87"/>
       <c r="AMF17" s="0"/>
       <c r="AMG17" s="0"/>
       <c r="AMH17" s="0"/>
@@ -5852,8 +5874,8 @@
       <c r="F18" s="45"/>
       <c r="G18" s="45"/>
       <c r="H18" s="45"/>
-      <c r="Q18" s="82"/>
-      <c r="T18" s="83"/>
+      <c r="Q18" s="86"/>
+      <c r="T18" s="87"/>
       <c r="AMF18" s="0"/>
       <c r="AMG18" s="0"/>
       <c r="AMH18" s="0"/>
@@ -5863,7 +5885,7 @@
     <row r="19" s="1" customFormat="true" ht="27.65" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A19" s="42"/>
       <c r="B19" s="42"/>
-      <c r="C19" s="48" t="s">
+      <c r="C19" s="50" t="s">
         <v>83</v>
       </c>
       <c r="D19" s="45" t="n">
@@ -5873,8 +5895,8 @@
       <c r="F19" s="45"/>
       <c r="G19" s="45"/>
       <c r="H19" s="45"/>
-      <c r="Q19" s="82"/>
-      <c r="T19" s="83"/>
+      <c r="Q19" s="86"/>
+      <c r="T19" s="87"/>
       <c r="AMF19" s="0"/>
       <c r="AMG19" s="0"/>
       <c r="AMH19" s="0"/>
@@ -5884,7 +5906,7 @@
     <row r="20" s="1" customFormat="true" ht="27.65" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A20" s="42"/>
       <c r="B20" s="42"/>
-      <c r="C20" s="47" t="s">
+      <c r="C20" s="51" t="s">
         <v>84</v>
       </c>
       <c r="D20" s="45" t="n">
@@ -5894,8 +5916,8 @@
       <c r="F20" s="45"/>
       <c r="G20" s="45"/>
       <c r="H20" s="45"/>
-      <c r="Q20" s="82"/>
-      <c r="T20" s="83"/>
+      <c r="Q20" s="86"/>
+      <c r="T20" s="87"/>
       <c r="AMF20" s="0"/>
       <c r="AMG20" s="0"/>
       <c r="AMH20" s="0"/>
@@ -5905,7 +5927,7 @@
     <row r="21" s="1" customFormat="true" ht="27.65" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A21" s="42"/>
       <c r="B21" s="42"/>
-      <c r="C21" s="48" t="s">
+      <c r="C21" s="50" t="s">
         <v>85</v>
       </c>
       <c r="D21" s="45" t="n">
@@ -5915,8 +5937,8 @@
       <c r="F21" s="45"/>
       <c r="G21" s="45"/>
       <c r="H21" s="45"/>
-      <c r="Q21" s="82"/>
-      <c r="T21" s="83"/>
+      <c r="Q21" s="86"/>
+      <c r="T21" s="87"/>
       <c r="AMF21" s="0"/>
       <c r="AMG21" s="0"/>
       <c r="AMH21" s="0"/>
@@ -5926,18 +5948,18 @@
     <row r="22" s="1" customFormat="true" ht="27.65" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A22" s="42"/>
       <c r="B22" s="42"/>
-      <c r="C22" s="49" t="s">
+      <c r="C22" s="52" t="s">
         <v>76</v>
       </c>
-      <c r="D22" s="50" t="n">
+      <c r="D22" s="53" t="n">
         <v>1</v>
       </c>
       <c r="E22" s="45"/>
       <c r="F22" s="45"/>
       <c r="G22" s="45"/>
       <c r="H22" s="45"/>
-      <c r="Q22" s="82"/>
-      <c r="T22" s="83"/>
+      <c r="Q22" s="86"/>
+      <c r="T22" s="87"/>
       <c r="AMF22" s="0"/>
       <c r="AMG22" s="0"/>
       <c r="AMH22" s="0"/>
@@ -5946,17 +5968,17 @@
     </row>
     <row r="23" s="1" customFormat="true" ht="34.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A23" s="42"/>
-      <c r="B23" s="51" t="s">
+      <c r="B23" s="54" t="s">
         <v>77</v>
       </c>
-      <c r="C23" s="51"/>
-      <c r="D23" s="51"/>
-      <c r="E23" s="51"/>
-      <c r="F23" s="51"/>
-      <c r="G23" s="51"/>
-      <c r="H23" s="51"/>
-      <c r="Q23" s="82"/>
-      <c r="T23" s="83"/>
+      <c r="C23" s="54"/>
+      <c r="D23" s="54"/>
+      <c r="E23" s="54"/>
+      <c r="F23" s="54"/>
+      <c r="G23" s="54"/>
+      <c r="H23" s="54"/>
+      <c r="Q23" s="86"/>
+      <c r="T23" s="87"/>
       <c r="AMF23" s="0"/>
       <c r="AMG23" s="0"/>
       <c r="AMH23" s="0"/>
@@ -5965,24 +5987,24 @@
     </row>
     <row r="24" s="1" customFormat="true" ht="34.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A24" s="42"/>
-      <c r="B24" s="52" t="s">
+      <c r="B24" s="55" t="s">
         <v>78</v>
       </c>
-      <c r="C24" s="53" t="n">
+      <c r="C24" s="56" t="n">
         <f aca="false">SUM(D11:D23)</f>
         <v>51</v>
       </c>
-      <c r="D24" s="52"/>
-      <c r="E24" s="52"/>
-      <c r="F24" s="52"/>
-      <c r="G24" s="52"/>
-      <c r="H24" s="52"/>
-      <c r="I24" s="46"/>
-      <c r="J24" s="46"/>
-      <c r="Q24" s="84"/>
-      <c r="R24" s="85"/>
-      <c r="S24" s="85"/>
-      <c r="T24" s="86"/>
+      <c r="D24" s="55"/>
+      <c r="E24" s="55"/>
+      <c r="F24" s="55"/>
+      <c r="G24" s="55"/>
+      <c r="H24" s="55"/>
+      <c r="I24" s="48"/>
+      <c r="J24" s="48"/>
+      <c r="Q24" s="88"/>
+      <c r="R24" s="89"/>
+      <c r="S24" s="89"/>
+      <c r="T24" s="90"/>
       <c r="AMF24" s="0"/>
       <c r="AMG24" s="0"/>
       <c r="AMH24" s="0"/>
@@ -5990,14 +6012,14 @@
       <c r="AMJ24" s="0"/>
     </row>
     <row r="25" s="1" customFormat="true" ht="8.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A25" s="60"/>
-      <c r="B25" s="61"/>
-      <c r="C25" s="62"/>
-      <c r="D25" s="63"/>
-      <c r="E25" s="63"/>
-      <c r="F25" s="63"/>
-      <c r="G25" s="63"/>
-      <c r="H25" s="64"/>
+      <c r="A25" s="64"/>
+      <c r="B25" s="65"/>
+      <c r="C25" s="66"/>
+      <c r="D25" s="67"/>
+      <c r="E25" s="67"/>
+      <c r="F25" s="67"/>
+      <c r="G25" s="67"/>
+      <c r="H25" s="68"/>
       <c r="AMF25" s="0"/>
       <c r="AMG25" s="0"/>
       <c r="AMH25" s="0"/>
@@ -6034,7 +6056,7 @@
   </sheetPr>
   <dimension ref="A1:AMJ1048576"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="65" zoomScaleNormal="65" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="75" zoomScaleNormal="75" zoomScalePageLayoutView="100" workbookViewId="0">
       <pane xSplit="2" ySplit="0" topLeftCell="C1" activePane="topRight" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
       <selection pane="topRight" activeCell="A11" activeCellId="0" sqref="A11"/>
@@ -6133,7 +6155,7 @@
       <c r="F7" s="37"/>
       <c r="G7" s="37"/>
       <c r="H7" s="37"/>
-      <c r="I7" s="75"/>
+      <c r="I7" s="79"/>
     </row>
     <row r="8" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="36"/>
@@ -6203,7 +6225,7 @@
       <c r="A11" s="42" t="s">
         <v>79</v>
       </c>
-      <c r="B11" s="81" t="s">
+      <c r="B11" s="85" t="s">
         <v>93</v>
       </c>
       <c r="C11" s="44" t="s">
@@ -6226,7 +6248,7 @@
       <c r="A12" s="42" t="s">
         <v>79</v>
       </c>
-      <c r="B12" s="81" t="s">
+      <c r="B12" s="85" t="s">
         <v>72</v>
       </c>
       <c r="C12" s="44" t="s">
@@ -6287,10 +6309,10 @@
       <c r="A15" s="42" t="s">
         <v>71</v>
       </c>
-      <c r="B15" s="81" t="s">
+      <c r="B15" s="85" t="s">
         <v>72</v>
       </c>
-      <c r="C15" s="47" t="s">
+      <c r="C15" s="51" t="s">
         <v>82</v>
       </c>
       <c r="D15" s="45" t="n">
@@ -6328,7 +6350,7 @@
     <row r="17" s="1" customFormat="true" ht="27.65" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A17" s="42"/>
       <c r="B17" s="42"/>
-      <c r="C17" s="48" t="s">
+      <c r="C17" s="50" t="s">
         <v>83</v>
       </c>
       <c r="D17" s="45" t="n">
@@ -6347,7 +6369,7 @@
     <row r="18" s="1" customFormat="true" ht="27.65" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A18" s="42"/>
       <c r="B18" s="42"/>
-      <c r="C18" s="47" t="s">
+      <c r="C18" s="51" t="s">
         <v>84</v>
       </c>
       <c r="D18" s="45" t="n">
@@ -6366,7 +6388,7 @@
     <row r="19" s="1" customFormat="true" ht="27.65" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A19" s="42"/>
       <c r="B19" s="42"/>
-      <c r="C19" s="48" t="s">
+      <c r="C19" s="50" t="s">
         <v>85</v>
       </c>
       <c r="D19" s="45" t="n">
@@ -6385,10 +6407,10 @@
     <row r="20" s="1" customFormat="true" ht="27.65" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A20" s="42"/>
       <c r="B20" s="42"/>
-      <c r="C20" s="49" t="s">
+      <c r="C20" s="52" t="s">
         <v>76</v>
       </c>
-      <c r="D20" s="50" t="n">
+      <c r="D20" s="53" t="n">
         <v>1</v>
       </c>
       <c r="E20" s="45"/>
@@ -6403,15 +6425,15 @@
     </row>
     <row r="21" s="1" customFormat="true" ht="34.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A21" s="42"/>
-      <c r="B21" s="51" t="s">
+      <c r="B21" s="54" t="s">
         <v>77</v>
       </c>
-      <c r="C21" s="51"/>
-      <c r="D21" s="51"/>
-      <c r="E21" s="51"/>
-      <c r="F21" s="51"/>
-      <c r="G21" s="51"/>
-      <c r="H21" s="51"/>
+      <c r="C21" s="54"/>
+      <c r="D21" s="54"/>
+      <c r="E21" s="54"/>
+      <c r="F21" s="54"/>
+      <c r="G21" s="54"/>
+      <c r="H21" s="54"/>
       <c r="AMF21" s="0"/>
       <c r="AMG21" s="0"/>
       <c r="AMH21" s="0"/>
@@ -6420,20 +6442,20 @@
     </row>
     <row r="22" s="1" customFormat="true" ht="34.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A22" s="42"/>
-      <c r="B22" s="52" t="s">
+      <c r="B22" s="55" t="s">
         <v>78</v>
       </c>
-      <c r="C22" s="53" t="n">
+      <c r="C22" s="56" t="n">
         <f aca="false">SUM(D11:D21)</f>
         <v>39</v>
       </c>
-      <c r="D22" s="52"/>
-      <c r="E22" s="52"/>
-      <c r="F22" s="52"/>
-      <c r="G22" s="52"/>
-      <c r="H22" s="52"/>
-      <c r="I22" s="46"/>
-      <c r="J22" s="46"/>
+      <c r="D22" s="55"/>
+      <c r="E22" s="55"/>
+      <c r="F22" s="55"/>
+      <c r="G22" s="55"/>
+      <c r="H22" s="55"/>
+      <c r="I22" s="48"/>
+      <c r="J22" s="48"/>
       <c r="AMF22" s="0"/>
       <c r="AMG22" s="0"/>
       <c r="AMH22" s="0"/>
@@ -6441,14 +6463,14 @@
       <c r="AMJ22" s="0"/>
     </row>
     <row r="23" s="1" customFormat="true" ht="8.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A23" s="60"/>
-      <c r="B23" s="61"/>
-      <c r="C23" s="62"/>
-      <c r="D23" s="63"/>
-      <c r="E23" s="63"/>
-      <c r="F23" s="63"/>
-      <c r="G23" s="63"/>
-      <c r="H23" s="64"/>
+      <c r="A23" s="64"/>
+      <c r="B23" s="65"/>
+      <c r="C23" s="66"/>
+      <c r="D23" s="67"/>
+      <c r="E23" s="67"/>
+      <c r="F23" s="67"/>
+      <c r="G23" s="67"/>
+      <c r="H23" s="68"/>
       <c r="AMF23" s="0"/>
       <c r="AMG23" s="0"/>
       <c r="AMH23" s="0"/>
@@ -6494,7 +6516,7 @@
   </sheetPr>
   <dimension ref="A1:AMJ1048576"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A4" colorId="64" zoomScale="65" zoomScaleNormal="65" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A4" colorId="64" zoomScale="75" zoomScaleNormal="75" zoomScalePageLayoutView="100" workbookViewId="0">
       <pane xSplit="2" ySplit="0" topLeftCell="C4" activePane="topRight" state="frozen"/>
       <selection pane="topLeft" activeCell="A4" activeCellId="0" sqref="A4"/>
       <selection pane="topRight" activeCell="A11" activeCellId="0" sqref="A11"/>
@@ -6593,7 +6615,7 @@
       <c r="F7" s="37"/>
       <c r="G7" s="37"/>
       <c r="H7" s="37"/>
-      <c r="I7" s="75"/>
+      <c r="I7" s="79"/>
     </row>
     <row r="8" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="36"/>
@@ -6663,7 +6685,7 @@
       <c r="A11" s="42" t="s">
         <v>79</v>
       </c>
-      <c r="B11" s="81" t="s">
+      <c r="B11" s="85" t="s">
         <v>94</v>
       </c>
       <c r="C11" s="44" t="s">
@@ -6686,7 +6708,7 @@
       <c r="A12" s="42" t="s">
         <v>79</v>
       </c>
-      <c r="B12" s="81" t="s">
+      <c r="B12" s="85" t="s">
         <v>72</v>
       </c>
       <c r="C12" s="44" t="s">
@@ -6747,10 +6769,10 @@
       <c r="A15" s="42" t="s">
         <v>71</v>
       </c>
-      <c r="B15" s="81" t="s">
+      <c r="B15" s="85" t="s">
         <v>72</v>
       </c>
-      <c r="C15" s="47" t="s">
+      <c r="C15" s="51" t="s">
         <v>82</v>
       </c>
       <c r="D15" s="45" t="n">
@@ -6788,7 +6810,7 @@
     <row r="17" s="1" customFormat="true" ht="27.65" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A17" s="42"/>
       <c r="B17" s="42"/>
-      <c r="C17" s="48" t="s">
+      <c r="C17" s="50" t="s">
         <v>83</v>
       </c>
       <c r="D17" s="45" t="n">
@@ -6807,7 +6829,7 @@
     <row r="18" s="1" customFormat="true" ht="27.65" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A18" s="42"/>
       <c r="B18" s="42"/>
-      <c r="C18" s="47" t="s">
+      <c r="C18" s="51" t="s">
         <v>84</v>
       </c>
       <c r="D18" s="45" t="n">
@@ -6826,7 +6848,7 @@
     <row r="19" s="1" customFormat="true" ht="27.65" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A19" s="42"/>
       <c r="B19" s="42"/>
-      <c r="C19" s="48" t="s">
+      <c r="C19" s="50" t="s">
         <v>85</v>
       </c>
       <c r="D19" s="45" t="n">
@@ -6845,10 +6867,10 @@
     <row r="20" s="1" customFormat="true" ht="27.65" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A20" s="42"/>
       <c r="B20" s="42"/>
-      <c r="C20" s="49" t="s">
+      <c r="C20" s="52" t="s">
         <v>76</v>
       </c>
-      <c r="D20" s="50" t="n">
+      <c r="D20" s="53" t="n">
         <v>1</v>
       </c>
       <c r="E20" s="45"/>
@@ -6863,15 +6885,15 @@
     </row>
     <row r="21" s="1" customFormat="true" ht="34.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A21" s="42"/>
-      <c r="B21" s="51" t="s">
+      <c r="B21" s="54" t="s">
         <v>77</v>
       </c>
-      <c r="C21" s="51"/>
-      <c r="D21" s="51"/>
-      <c r="E21" s="51"/>
-      <c r="F21" s="51"/>
-      <c r="G21" s="51"/>
-      <c r="H21" s="51"/>
+      <c r="C21" s="54"/>
+      <c r="D21" s="54"/>
+      <c r="E21" s="54"/>
+      <c r="F21" s="54"/>
+      <c r="G21" s="54"/>
+      <c r="H21" s="54"/>
       <c r="AMF21" s="0"/>
       <c r="AMG21" s="0"/>
       <c r="AMH21" s="0"/>
@@ -6880,20 +6902,20 @@
     </row>
     <row r="22" s="1" customFormat="true" ht="34.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A22" s="42"/>
-      <c r="B22" s="52" t="s">
+      <c r="B22" s="55" t="s">
         <v>78</v>
       </c>
-      <c r="C22" s="53" t="n">
+      <c r="C22" s="56" t="n">
         <f aca="false">SUM(D11:D21)</f>
         <v>39</v>
       </c>
-      <c r="D22" s="52"/>
-      <c r="E22" s="52"/>
-      <c r="F22" s="52"/>
-      <c r="G22" s="52"/>
-      <c r="H22" s="52"/>
-      <c r="I22" s="46"/>
-      <c r="J22" s="46"/>
+      <c r="D22" s="55"/>
+      <c r="E22" s="55"/>
+      <c r="F22" s="55"/>
+      <c r="G22" s="55"/>
+      <c r="H22" s="55"/>
+      <c r="I22" s="48"/>
+      <c r="J22" s="48"/>
       <c r="AMF22" s="0"/>
       <c r="AMG22" s="0"/>
       <c r="AMH22" s="0"/>
@@ -6901,14 +6923,14 @@
       <c r="AMJ22" s="0"/>
     </row>
     <row r="23" s="1" customFormat="true" ht="8.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A23" s="60"/>
-      <c r="B23" s="61"/>
-      <c r="C23" s="62"/>
-      <c r="D23" s="63"/>
-      <c r="E23" s="63"/>
-      <c r="F23" s="63"/>
-      <c r="G23" s="63"/>
-      <c r="H23" s="64"/>
+      <c r="A23" s="64"/>
+      <c r="B23" s="65"/>
+      <c r="C23" s="66"/>
+      <c r="D23" s="67"/>
+      <c r="E23" s="67"/>
+      <c r="F23" s="67"/>
+      <c r="G23" s="67"/>
+      <c r="H23" s="68"/>
       <c r="AMF23" s="0"/>
       <c r="AMG23" s="0"/>
       <c r="AMH23" s="0"/>

</xml_diff>

<commit_message>
Version sprint 1 à terminer
</commit_message>
<xml_diff>
--- a/Tableau_SCRUM_B3D.xlsx
+++ b/Tableau_SCRUM_B3D.xlsx
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="244" uniqueCount="95">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="250" uniqueCount="107">
   <si>
     <t xml:space="preserve">PRODUCT  BACKLOG – Création site B3D</t>
   </si>
@@ -283,13 +283,48 @@
     <t xml:space="preserve">Maquette graphique</t>
   </si>
   <si>
+    <t xml:space="preserve">création logo</t>
+  </si>
+  <si>
     <t xml:space="preserve">étude et prise en main des effets parallaxe</t>
   </si>
   <si>
-    <t xml:space="preserve">intégration du menu + logo</t>
-  </si>
-  <si>
-    <t xml:space="preserve">intégration footer + contact</t>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">création </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve"> du menu + intégration logo</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">Création -</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve"> footer + contact</t>
+    </r>
   </si>
   <si>
     <t xml:space="preserve">3ème</t>
@@ -300,13 +335,61 @@
 Flat design &amp; Effets parallaxe</t>
   </si>
   <si>
-    <t xml:space="preserve">Intégration – page accueil</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Intégration – page société</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Intégration – page produits</t>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">Création </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve"> – page accueil</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">Création </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve"> – page société</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">Création </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve"> – page produits</t>
+    </r>
   </si>
   <si>
     <t xml:space="preserve">intégration de photos</t>
@@ -370,7 +453,7 @@
     <t xml:space="preserve">Maquette fonctionnelle – tablette</t>
   </si>
   <si>
-    <t xml:space="preserve">Intégration - ergonomie et responsive design</t>
+    <t xml:space="preserve">création « « pages produits responsive design</t>
   </si>
   <si>
     <t xml:space="preserve">intégration du logo</t>
@@ -426,6 +509,9 @@
       <t xml:space="preserve">)
 Page de contact</t>
     </r>
+  </si>
+  <si>
+    <t xml:space="preserve">Création – développement pages responsive design</t>
   </si>
   <si>
     <t xml:space="preserve">Burdown Chart - Refonte du site www.corrtech.fr</t>
@@ -502,6 +588,36 @@
     </r>
   </si>
   <si>
+    <t xml:space="preserve">Intégration - ergonomie et responsive design</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Jour 1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Jour 2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Jour 3</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Jour 4</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Jour 5</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Jour 6</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Jour 7</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Jour 8</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Jour 9</t>
+  </si>
+  <si>
     <r>
       <rPr>
         <sz val="11"/>
@@ -622,7 +738,7 @@
     <numFmt numFmtId="164" formatCode="General"/>
     <numFmt numFmtId="165" formatCode="#,##0.00"/>
   </numFmts>
-  <fonts count="29">
+  <fonts count="30">
     <font>
       <sz val="10"/>
       <color rgb="FF000000"/>
@@ -750,6 +866,11 @@
       <name val="Calibri"/>
       <family val="2"/>
       <charset val="1"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <name val="Calibri"/>
+      <family val="2"/>
     </font>
     <font>
       <sz val="11"/>
@@ -1060,7 +1181,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="91">
+  <cellXfs count="93">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -1237,27 +1358,79 @@
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
+    <xf numFmtId="164" fontId="9" fillId="7" borderId="3" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="9" fillId="7" borderId="3" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="9" fillId="3" borderId="3" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="9" fillId="3" borderId="3" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="19" fillId="3" borderId="9" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="19" fillId="0" borderId="3" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="9" fillId="0" borderId="3" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="9" fillId="3" borderId="3" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="9" fillId="5" borderId="3" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="14" fillId="0" borderId="3" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="14" fillId="0" borderId="3" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="right" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="17" fillId="0" borderId="3" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="20" fillId="2" borderId="6" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="21" fillId="2" borderId="3" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="21" fillId="2" borderId="3" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="right" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="20" fillId="2" borderId="3" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
     <xf numFmtId="164" fontId="9" fillId="0" borderId="3" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="9" fillId="0" borderId="3" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="9" fillId="7" borderId="3" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="9" fillId="7" borderId="3" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="9" fillId="7" borderId="9" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="9" fillId="0" borderId="9" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -1265,50 +1438,6 @@
       <alignment horizontal="left" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="9" fillId="0" borderId="9" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="9" fillId="3" borderId="3" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="9" fillId="3" borderId="3" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="9" fillId="5" borderId="3" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="14" fillId="0" borderId="3" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="14" fillId="0" borderId="3" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="right" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="17" fillId="0" borderId="3" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="19" fillId="2" borderId="6" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="20" fillId="2" borderId="3" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="20" fillId="2" borderId="3" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="right" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="19" fillId="2" borderId="3" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
     <xf numFmtId="164" fontId="7" fillId="5" borderId="3" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -1341,31 +1470,31 @@
       <alignment horizontal="general" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="21" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
     <xf numFmtId="164" fontId="22" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="23" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="24" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="24" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="25" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="25" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="26" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="23" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="24" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="left" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="26" fillId="8" borderId="8" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="27" fillId="8" borderId="8" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -1377,7 +1506,7 @@
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="28" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="29" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -1483,8 +1612,8 @@
       <rgbColor rgb="FFFF9900"/>
       <rgbColor rgb="FFFF420E"/>
       <rgbColor rgb="FF666699"/>
-      <rgbColor rgb="FF969696"/>
-      <rgbColor rgb="FF003366"/>
+      <rgbColor rgb="FFB3B3B3"/>
+      <rgbColor rgb="FF004586"/>
       <rgbColor rgb="FF3D85C6"/>
       <rgbColor rgb="FF003300"/>
       <rgbColor rgb="FF333300"/>
@@ -1508,10 +1637,10 @@
           <c:layoutTarget val="inner"/>
           <c:xMode val="edge"/>
           <c:yMode val="edge"/>
-          <c:x val="0.134035569803832"/>
-          <c:y val="0.196514116807665"/>
-          <c:w val="0.737195633921075"/>
-          <c:h val="0.672102741820406"/>
+          <c:x val="0.134045801526718"/>
+          <c:y val="0.196534148827727"/>
+          <c:w val="0.737175572519084"/>
+          <c:h val="0.672069317023445"/>
         </c:manualLayout>
       </c:layout>
       <c:lineChart>
@@ -1873,11 +2002,11 @@
           </c:spPr>
         </c:hiLowLines>
         <c:marker val="1"/>
-        <c:axId val="70068314"/>
-        <c:axId val="6673470"/>
+        <c:axId val="87012736"/>
+        <c:axId val="58809470"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="70068314"/>
+        <c:axId val="87012736"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1925,14 +2054,14 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="6673470"/>
+        <c:crossAx val="58809470"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="6673470"/>
+        <c:axId val="58809470"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1976,7 +2105,7 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="70068314"/>
+        <c:crossAx val="87012736"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -2233,11 +2362,11 @@
           </c:spPr>
         </c:hiLowLines>
         <c:marker val="1"/>
-        <c:axId val="7754835"/>
-        <c:axId val="54543078"/>
+        <c:axId val="79975181"/>
+        <c:axId val="27970310"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="7754835"/>
+        <c:axId val="79975181"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2263,14 +2392,14 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="54543078"/>
+        <c:crossAx val="27970310"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="54543078"/>
+        <c:axId val="27970310"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2305,7 +2434,7 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="7754835"/>
+        <c:crossAx val="79975181"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -2363,40 +2492,38 @@
           <c:order val="0"/>
           <c:tx>
             <c:strRef>
-              <c:f>'Sprint 2'!$B$9</c:f>
+              <c:f>'Sprint 2'!$C$9</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v/>
+                  <c:v>Trajectoire idéale</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
           </c:tx>
           <c:spPr>
             <a:solidFill>
-              <a:srgbClr val="3366cc"/>
+              <a:srgbClr val="004586"/>
             </a:solidFill>
-            <a:ln w="19080">
+            <a:ln w="28800">
               <a:solidFill>
-                <a:srgbClr val="3366cc"/>
+                <a:srgbClr val="004586"/>
               </a:solidFill>
               <a:round/>
             </a:ln>
           </c:spPr>
           <c:marker>
-            <c:symbol val="circle"/>
-            <c:size val="10"/>
+            <c:symbol val="square"/>
+            <c:size val="8"/>
             <c:spPr>
               <a:solidFill>
-                <a:srgbClr val="3366cc"/>
+                <a:srgbClr val="004586"/>
               </a:solidFill>
             </c:spPr>
           </c:marker>
           <c:dLbls>
-            <c:numFmt formatCode="General" sourceLinked="1"/>
-            <c:dLblPos val="r"/>
             <c:showLegendKey val="0"/>
-            <c:showVal val="1"/>
+            <c:showVal val="0"/>
             <c:showCatName val="0"/>
             <c:showSerName val="0"/>
             <c:showPercent val="0"/>
@@ -2404,46 +2531,76 @@
           </c:dLbls>
           <c:cat>
             <c:strRef>
-              <c:f>'Sprint 2'!$C$8:$G$8</c:f>
+              <c:f>'Sprint 2'!$D$8:$M$8</c:f>
               <c:strCache>
-                <c:ptCount val="5"/>
+                <c:ptCount val="10"/>
                 <c:pt idx="0">
-                  <c:v>Jours d'itération</c:v>
+                  <c:v>Estimation</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>Jeu 6 dec.</c:v>
+                  <c:v>Jour 1</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>Jeu 13 dec.</c:v>
+                  <c:v>Jour 2</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>Jeu 20 dec.</c:v>
+                  <c:v>Jour 3</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>Jeu 3 janv.</c:v>
+                  <c:v>Jour 4</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>Jour 5</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>Jour 6</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>Jour 7</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>Jour 8</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>Jour 9</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>'Sprint 2'!$C$9:$G$9</c:f>
+              <c:f>'Sprint 2'!$D$9:$M$9</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="5"/>
+                <c:ptCount val="10"/>
                 <c:pt idx="0">
-                  <c:v/>
+                  <c:v>63</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v/>
+                  <c:v>56</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>0</c:v>
+                  <c:v>49</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>0</c:v>
+                  <c:v>42</c:v>
                 </c:pt>
                 <c:pt idx="4">
+                  <c:v>35</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>28</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>21</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>14</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>7</c:v>
+                </c:pt>
+                <c:pt idx="9">
                   <c:v>0</c:v>
                 </c:pt>
               </c:numCache>
@@ -2456,40 +2613,38 @@
           <c:order val="1"/>
           <c:tx>
             <c:strRef>
-              <c:f>'Sprint 2'!$B$10</c:f>
+              <c:f>'Sprint 2'!$C$10</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v/>
+                  <c:v>Trajectoire réelle</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
           </c:tx>
           <c:spPr>
             <a:solidFill>
-              <a:srgbClr val="dc3912"/>
+              <a:srgbClr val="ff420e"/>
             </a:solidFill>
-            <a:ln w="19080">
+            <a:ln w="28800">
               <a:solidFill>
-                <a:srgbClr val="dc3912"/>
+                <a:srgbClr val="ff420e"/>
               </a:solidFill>
               <a:round/>
             </a:ln>
           </c:spPr>
           <c:marker>
-            <c:symbol val="circle"/>
-            <c:size val="10"/>
+            <c:symbol val="diamond"/>
+            <c:size val="8"/>
             <c:spPr>
               <a:solidFill>
-                <a:srgbClr val="dc3912"/>
+                <a:srgbClr val="ff420e"/>
               </a:solidFill>
             </c:spPr>
           </c:marker>
           <c:dLbls>
-            <c:numFmt formatCode="General" sourceLinked="1"/>
-            <c:dLblPos val="r"/>
             <c:showLegendKey val="0"/>
-            <c:showVal val="1"/>
+            <c:showVal val="0"/>
             <c:showCatName val="0"/>
             <c:showSerName val="0"/>
             <c:showPercent val="0"/>
@@ -2497,47 +2652,77 @@
           </c:dLbls>
           <c:cat>
             <c:strRef>
-              <c:f>'Sprint 2'!$C$8:$G$8</c:f>
+              <c:f>'Sprint 2'!$D$8:$M$8</c:f>
               <c:strCache>
-                <c:ptCount val="5"/>
+                <c:ptCount val="10"/>
                 <c:pt idx="0">
-                  <c:v>Jours d'itération</c:v>
+                  <c:v>Estimation</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>Jeu 6 dec.</c:v>
+                  <c:v>Jour 1</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>Jeu 13 dec.</c:v>
+                  <c:v>Jour 2</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>Jeu 20 dec.</c:v>
+                  <c:v>Jour 3</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>Jeu 3 janv.</c:v>
+                  <c:v>Jour 4</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>Jour 5</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>Jour 6</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>Jour 7</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>Jour 8</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>Jour 9</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>'Sprint 2'!$C$10:$G$10</c:f>
+              <c:f>'Sprint 2'!$D$10:$M$10</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="5"/>
+                <c:ptCount val="10"/>
                 <c:pt idx="0">
-                  <c:v/>
+                  <c:v>38</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v/>
+                  <c:v>31</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v/>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v/>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v/>
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>0</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2552,23 +2737,25 @@
           </c:spPr>
         </c:hiLowLines>
         <c:marker val="1"/>
-        <c:axId val="30328266"/>
-        <c:axId val="53304297"/>
+        <c:axId val="59960415"/>
+        <c:axId val="41017333"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="30328266"/>
+        <c:axId val="59960415"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:delete val="0"/>
         <c:axPos val="b"/>
         <c:numFmt formatCode="General" sourceLinked="1"/>
-        <c:majorTickMark val="cross"/>
-        <c:minorTickMark val="cross"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
         <c:spPr>
           <a:ln>
-            <a:noFill/>
+            <a:solidFill>
+              <a:srgbClr val="b3b3b3"/>
+            </a:solidFill>
           </a:ln>
         </c:spPr>
         <c:txPr>
@@ -2582,14 +2769,14 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="53304297"/>
+        <c:crossAx val="41017333"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="53304297"/>
+        <c:axId val="41017333"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2599,18 +2786,20 @@
           <c:spPr>
             <a:ln>
               <a:solidFill>
-                <a:srgbClr val="b7b7b7"/>
+                <a:srgbClr val="b3b3b3"/>
               </a:solidFill>
             </a:ln>
           </c:spPr>
         </c:majorGridlines>
-        <c:numFmt formatCode="General" sourceLinked="0"/>
-        <c:majorTickMark val="cross"/>
-        <c:minorTickMark val="cross"/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
         <c:spPr>
-          <a:ln w="47520">
-            <a:noFill/>
+          <a:ln>
+            <a:solidFill>
+              <a:srgbClr val="b3b3b3"/>
+            </a:solidFill>
           </a:ln>
         </c:spPr>
         <c:txPr>
@@ -2624,14 +2813,16 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="30328266"/>
+        <c:crossAx val="59960415"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:spPr>
         <a:noFill/>
         <a:ln>
-          <a:noFill/>
+          <a:solidFill>
+            <a:srgbClr val="b3b3b3"/>
+          </a:solidFill>
         </a:ln>
       </c:spPr>
     </c:plotArea>
@@ -2657,10 +2848,12 @@
       </c:txPr>
     </c:legend>
     <c:plotVisOnly val="1"/>
-    <c:dispBlanksAs val="zero"/>
+    <c:dispBlanksAs val="gap"/>
   </c:chart>
   <c:spPr>
-    <a:noFill/>
+    <a:solidFill>
+      <a:srgbClr val="ffffff"/>
+    </a:solidFill>
     <a:ln>
       <a:noFill/>
     </a:ln>
@@ -2871,11 +3064,11 @@
           </c:spPr>
         </c:hiLowLines>
         <c:marker val="1"/>
-        <c:axId val="67935151"/>
-        <c:axId val="99656486"/>
+        <c:axId val="57656922"/>
+        <c:axId val="91614892"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="67935151"/>
+        <c:axId val="57656922"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2901,14 +3094,14 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="99656486"/>
+        <c:crossAx val="91614892"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="99656486"/>
+        <c:axId val="91614892"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2943,7 +3136,7 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="67935151"/>
+        <c:crossAx val="57656922"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -2998,9 +3191,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>5</xdr:col>
-      <xdr:colOff>915120</xdr:colOff>
+      <xdr:colOff>914760</xdr:colOff>
       <xdr:row>20</xdr:row>
-      <xdr:rowOff>205200</xdr:rowOff>
+      <xdr:rowOff>204840</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame>
       <xdr:nvGraphicFramePr>
@@ -3009,7 +3202,7 @@
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
         <a:off x="1718280" y="3404520"/>
-        <a:ext cx="4716000" cy="3531600"/>
+        <a:ext cx="4715640" cy="3531240"/>
       </xdr:xfrm>
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
@@ -3033,9 +3226,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>12</xdr:col>
-      <xdr:colOff>76320</xdr:colOff>
+      <xdr:colOff>75960</xdr:colOff>
       <xdr:row>22</xdr:row>
-      <xdr:rowOff>297360</xdr:rowOff>
+      <xdr:rowOff>297000</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame>
       <xdr:nvGraphicFramePr>
@@ -3044,7 +3237,7 @@
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
         <a:off x="13459680" y="1436040"/>
-        <a:ext cx="4093560" cy="5615640"/>
+        <a:ext cx="4093200" cy="5615280"/>
       </xdr:xfrm>
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
@@ -3061,25 +3254,25 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
-      <xdr:col>8</xdr:col>
-      <xdr:colOff>54360</xdr:colOff>
-      <xdr:row>5</xdr:row>
-      <xdr:rowOff>124920</xdr:rowOff>
+      <xdr:col>13</xdr:col>
+      <xdr:colOff>146520</xdr:colOff>
+      <xdr:row>11</xdr:row>
+      <xdr:rowOff>10440</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>12</xdr:col>
-      <xdr:colOff>77040</xdr:colOff>
-      <xdr:row>17</xdr:row>
-      <xdr:rowOff>108720</xdr:rowOff>
+      <xdr:col>18</xdr:col>
+      <xdr:colOff>816840</xdr:colOff>
+      <xdr:row>20</xdr:row>
+      <xdr:rowOff>90000</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame>
       <xdr:nvGraphicFramePr>
-        <xdr:cNvPr id="2" name="Chart 2"/>
+        <xdr:cNvPr id="2" name=""/>
         <xdr:cNvGraphicFramePr/>
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
-        <a:off x="13459680" y="1436040"/>
-        <a:ext cx="4094280" cy="3318120"/>
+        <a:off x="18641520" y="2549160"/>
+        <a:ext cx="5759640" cy="3239640"/>
       </xdr:xfrm>
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
@@ -3103,9 +3296,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>12</xdr:col>
-      <xdr:colOff>75960</xdr:colOff>
+      <xdr:colOff>75600</xdr:colOff>
       <xdr:row>17</xdr:row>
-      <xdr:rowOff>186120</xdr:rowOff>
+      <xdr:rowOff>185760</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame>
       <xdr:nvGraphicFramePr>
@@ -3114,7 +3307,7 @@
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
         <a:off x="13459680" y="1436040"/>
-        <a:ext cx="4093200" cy="3395520"/>
+        <a:ext cx="4092840" cy="3395160"/>
       </xdr:xfrm>
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
@@ -4485,12 +4678,12 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="true"/>
   </sheetPr>
-  <dimension ref="A1:AMJ52"/>
+  <dimension ref="A1:AMJ53"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="75" zoomScaleNormal="75" zoomScalePageLayoutView="100" workbookViewId="0">
-      <pane xSplit="0" ySplit="9" topLeftCell="D19" activePane="bottomLeft" state="frozen"/>
+      <pane xSplit="0" ySplit="9" topLeftCell="D37" activePane="bottomLeft" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-      <selection pane="bottomLeft" activeCell="F25" activeCellId="0" sqref="F25"/>
+      <selection pane="bottomLeft" activeCell="C41" activeCellId="0" sqref="C41"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -4625,7 +4818,7 @@
         <v>58</v>
       </c>
       <c r="D9" s="41" t="e">
-        <f aca="false">SUM(D40:D43,#REF!)</f>
+        <f aca="false">SUM(D41:D44,#REF!)</f>
         <v>#REF!</v>
       </c>
       <c r="E9" s="41" t="n">
@@ -4707,76 +4900,76 @@
     <row r="13" customFormat="false" ht="26.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A13" s="42"/>
       <c r="B13" s="42"/>
-      <c r="C13" s="46" t="s">
+      <c r="C13" s="44" t="s">
         <v>64</v>
       </c>
-      <c r="D13" s="47" t="n">
+      <c r="D13" s="45" t="n">
         <v>6</v>
       </c>
-      <c r="E13" s="47" t="n">
+      <c r="E13" s="45" t="n">
         <v>0</v>
       </c>
-      <c r="F13" s="47" t="n">
+      <c r="F13" s="45" t="n">
         <v>0</v>
       </c>
-      <c r="G13" s="47"/>
-      <c r="H13" s="47"/>
+      <c r="G13" s="45"/>
+      <c r="H13" s="45"/>
     </row>
     <row r="14" customFormat="false" ht="26.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A14" s="42"/>
       <c r="B14" s="43"/>
-      <c r="C14" s="46" t="s">
+      <c r="C14" s="44" t="s">
         <v>65</v>
       </c>
-      <c r="D14" s="47" t="n">
+      <c r="D14" s="45" t="n">
         <v>2</v>
       </c>
-      <c r="E14" s="47" t="n">
+      <c r="E14" s="45" t="n">
         <v>2</v>
       </c>
-      <c r="F14" s="47" t="n">
+      <c r="F14" s="45" t="n">
         <v>0</v>
       </c>
-      <c r="G14" s="47"/>
-      <c r="H14" s="47"/>
+      <c r="G14" s="45"/>
+      <c r="H14" s="45"/>
     </row>
     <row r="15" customFormat="false" ht="26.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A15" s="42"/>
       <c r="B15" s="42"/>
-      <c r="C15" s="46" t="s">
+      <c r="C15" s="44" t="s">
         <v>66</v>
       </c>
-      <c r="D15" s="47" t="n">
+      <c r="D15" s="45" t="n">
         <v>2</v>
       </c>
-      <c r="E15" s="47" t="n">
+      <c r="E15" s="45" t="n">
         <v>0</v>
       </c>
-      <c r="F15" s="47" t="n">
+      <c r="F15" s="45" t="n">
         <v>0</v>
       </c>
-      <c r="G15" s="47"/>
-      <c r="H15" s="47"/>
+      <c r="G15" s="45"/>
+      <c r="H15" s="45"/>
     </row>
     <row r="16" customFormat="false" ht="26.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A16" s="42"/>
       <c r="B16" s="42"/>
-      <c r="C16" s="46" t="s">
+      <c r="C16" s="44" t="s">
         <v>67</v>
       </c>
-      <c r="D16" s="47" t="n">
+      <c r="D16" s="45" t="n">
         <v>12</v>
       </c>
-      <c r="E16" s="47" t="n">
+      <c r="E16" s="45" t="n">
         <v>6</v>
       </c>
-      <c r="F16" s="47" t="n">
+      <c r="F16" s="45" t="n">
         <v>0</v>
       </c>
-      <c r="G16" s="47"/>
-      <c r="H16" s="47"/>
-      <c r="I16" s="48"/>
-      <c r="J16" s="48"/>
+      <c r="G16" s="45"/>
+      <c r="H16" s="45"/>
+      <c r="I16" s="46"/>
+      <c r="J16" s="46"/>
     </row>
     <row r="17" customFormat="false" ht="26.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A17" s="42"/>
@@ -4784,573 +4977,587 @@
       <c r="C17" s="44" t="s">
         <v>68</v>
       </c>
-      <c r="D17" s="45" t="n">
-        <v>4</v>
-      </c>
-      <c r="E17" s="45" t="n">
-        <v>4</v>
-      </c>
-      <c r="F17" s="45" t="n">
-        <v>4</v>
-      </c>
+      <c r="D17" s="45"/>
+      <c r="E17" s="45"/>
+      <c r="F17" s="45"/>
       <c r="G17" s="45"/>
       <c r="H17" s="45"/>
+      <c r="I17" s="46"/>
+      <c r="J17" s="46"/>
     </row>
     <row r="18" customFormat="false" ht="26.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A18" s="42"/>
       <c r="B18" s="42"/>
-      <c r="C18" s="49" t="s">
+      <c r="C18" s="47" t="s">
         <v>69</v>
       </c>
-      <c r="D18" s="47" t="n">
-        <v>1</v>
-      </c>
-      <c r="E18" s="47" t="n">
-        <v>1</v>
-      </c>
-      <c r="F18" s="47" t="n">
-        <v>0</v>
-      </c>
-      <c r="G18" s="47"/>
-      <c r="H18" s="47"/>
+      <c r="D18" s="48" t="n">
+        <v>4</v>
+      </c>
+      <c r="E18" s="48" t="n">
+        <v>4</v>
+      </c>
+      <c r="F18" s="48" t="n">
+        <v>4</v>
+      </c>
+      <c r="G18" s="48"/>
+      <c r="H18" s="48"/>
     </row>
     <row r="19" customFormat="false" ht="26.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A19" s="42"/>
       <c r="B19" s="42"/>
-      <c r="C19" s="50" t="s">
+      <c r="C19" s="49" t="s">
         <v>70</v>
       </c>
-      <c r="D19" s="45" t="n">
+      <c r="D19" s="48" t="n">
+        <v>1</v>
+      </c>
+      <c r="E19" s="48" t="n">
+        <v>1</v>
+      </c>
+      <c r="F19" s="48" t="n">
+        <v>0</v>
+      </c>
+      <c r="G19" s="48"/>
+      <c r="H19" s="48"/>
+    </row>
+    <row r="20" customFormat="false" ht="26.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A20" s="42"/>
+      <c r="B20" s="42"/>
+      <c r="C20" s="50" t="s">
+        <v>71</v>
+      </c>
+      <c r="D20" s="51" t="n">
         <v>2</v>
       </c>
-      <c r="E19" s="45" t="n">
+      <c r="E20" s="51" t="n">
         <v>1</v>
       </c>
-      <c r="F19" s="45" t="n">
+      <c r="F20" s="51" t="n">
         <v>2</v>
       </c>
-      <c r="G19" s="45"/>
-      <c r="H19" s="45"/>
-    </row>
-    <row r="20" customFormat="false" ht="26.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A20" s="42" t="s">
-        <v>71</v>
-      </c>
-      <c r="B20" s="43" t="s">
-        <v>72</v>
-      </c>
-      <c r="C20" s="49" t="s">
-        <v>73</v>
-      </c>
-      <c r="D20" s="47" t="n">
-        <v>4</v>
-      </c>
-      <c r="E20" s="47" t="n">
-        <v>0</v>
-      </c>
-      <c r="F20" s="47" t="n">
-        <v>0</v>
-      </c>
-      <c r="G20" s="47"/>
-      <c r="H20" s="47"/>
+      <c r="G20" s="51"/>
+      <c r="H20" s="51"/>
     </row>
     <row r="21" customFormat="false" ht="26.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A21" s="42" t="s">
-        <v>71</v>
+        <v>72</v>
       </c>
       <c r="B21" s="43" t="s">
-        <v>72</v>
-      </c>
-      <c r="C21" s="51" t="s">
+        <v>73</v>
+      </c>
+      <c r="C21" s="49" t="s">
         <v>74</v>
       </c>
-      <c r="D21" s="45" t="n">
-        <v>8</v>
-      </c>
-      <c r="E21" s="45" t="n">
-        <v>8</v>
-      </c>
-      <c r="F21" s="45" t="n">
-        <v>2</v>
-      </c>
-      <c r="G21" s="45"/>
-      <c r="H21" s="45"/>
+      <c r="D21" s="48" t="n">
+        <v>4</v>
+      </c>
+      <c r="E21" s="48" t="n">
+        <v>0</v>
+      </c>
+      <c r="F21" s="48" t="n">
+        <v>0</v>
+      </c>
+      <c r="G21" s="48"/>
+      <c r="H21" s="48"/>
     </row>
     <row r="22" customFormat="false" ht="26.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A22" s="42" t="s">
-        <v>71</v>
+        <v>72</v>
       </c>
       <c r="B22" s="43" t="s">
+        <v>73</v>
+      </c>
+      <c r="C22" s="49" t="s">
+        <v>75</v>
+      </c>
+      <c r="D22" s="48" t="n">
+        <v>8</v>
+      </c>
+      <c r="E22" s="48" t="n">
+        <v>8</v>
+      </c>
+      <c r="F22" s="48" t="n">
+        <v>2</v>
+      </c>
+      <c r="G22" s="48"/>
+      <c r="H22" s="48"/>
+    </row>
+    <row r="23" customFormat="false" ht="26.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A23" s="42" t="s">
         <v>72</v>
       </c>
-      <c r="C22" s="51" t="s">
-        <v>75</v>
-      </c>
-      <c r="D22" s="45" t="n">
+      <c r="B23" s="43" t="s">
+        <v>73</v>
+      </c>
+      <c r="C23" s="49" t="s">
+        <v>76</v>
+      </c>
+      <c r="D23" s="48" t="n">
         <v>8</v>
       </c>
-      <c r="E22" s="45" t="n">
+      <c r="E23" s="48" t="n">
         <v>8</v>
       </c>
-      <c r="F22" s="45" t="n">
+      <c r="F23" s="48" t="n">
         <v>8</v>
       </c>
-      <c r="G22" s="45"/>
-      <c r="H22" s="45"/>
-    </row>
-    <row r="23" customFormat="false" ht="26.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A23" s="42"/>
-      <c r="B23" s="42"/>
-      <c r="C23" s="52" t="s">
-        <v>76</v>
-      </c>
-      <c r="D23" s="53" t="n">
+      <c r="G23" s="48"/>
+      <c r="H23" s="48"/>
+    </row>
+    <row r="24" customFormat="false" ht="26.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A24" s="42"/>
+      <c r="B24" s="42"/>
+      <c r="C24" s="52" t="s">
+        <v>77</v>
+      </c>
+      <c r="D24" s="48" t="n">
         <v>1</v>
       </c>
-      <c r="E23" s="45" t="n">
+      <c r="E24" s="48" t="n">
         <v>1</v>
       </c>
-      <c r="F23" s="45" t="n">
+      <c r="F24" s="48" t="n">
         <v>1</v>
       </c>
-      <c r="G23" s="45"/>
-      <c r="H23" s="45"/>
-      <c r="I23" s="48"/>
-      <c r="J23" s="48"/>
-    </row>
-    <row r="24" customFormat="false" ht="27.65" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A24" s="42"/>
-      <c r="B24" s="54" t="s">
-        <v>77</v>
-      </c>
-      <c r="C24" s="54"/>
-      <c r="D24" s="54"/>
-      <c r="E24" s="54"/>
-      <c r="F24" s="54"/>
-      <c r="G24" s="54"/>
-      <c r="H24" s="54"/>
+      <c r="G24" s="48"/>
+      <c r="H24" s="48"/>
+      <c r="I24" s="46"/>
+      <c r="J24" s="46"/>
     </row>
     <row r="25" customFormat="false" ht="27.65" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A25" s="42"/>
-      <c r="B25" s="55" t="s">
+      <c r="B25" s="53" t="s">
         <v>78</v>
       </c>
-      <c r="C25" s="56" t="n">
+      <c r="C25" s="53"/>
+      <c r="D25" s="53"/>
+      <c r="E25" s="53"/>
+      <c r="F25" s="53"/>
+      <c r="G25" s="53"/>
+      <c r="H25" s="53"/>
+    </row>
+    <row r="26" customFormat="false" ht="27.65" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A26" s="42"/>
+      <c r="B26" s="54" t="s">
+        <v>79</v>
+      </c>
+      <c r="C26" s="55" t="n">
+        <f aca="false">SUM(D11:D25)</f>
+        <v>62</v>
+      </c>
+      <c r="D26" s="56" t="n">
         <f aca="false">SUM(D11:D24)</f>
         <v>62</v>
       </c>
-      <c r="D25" s="57" t="n">
-        <f aca="false">SUM(D11:D23)</f>
-        <v>62</v>
-      </c>
-      <c r="E25" s="57" t="n">
-        <f aca="false">SUM(E11:E23)</f>
+      <c r="E26" s="56" t="n">
+        <f aca="false">SUM(E11:E24)</f>
         <v>37</v>
       </c>
-      <c r="F25" s="57" t="n">
-        <f aca="false">SUM(F14:F23)</f>
+      <c r="F26" s="56" t="n">
+        <f aca="false">SUM(F14:F24)</f>
         <v>17</v>
       </c>
-      <c r="G25" s="57" t="n">
-        <f aca="false">SUM(G14:G23)</f>
+      <c r="G26" s="56" t="n">
+        <f aca="false">SUM(G14:G24)</f>
         <v>0</v>
       </c>
-      <c r="H25" s="57" t="n">
-        <f aca="false">SUM(H14:H23)</f>
+      <c r="H26" s="56" t="n">
+        <f aca="false">SUM(H14:H24)</f>
         <v>0</v>
       </c>
     </row>
-    <row r="26" customFormat="false" ht="11.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A26" s="58"/>
-      <c r="B26" s="59"/>
-      <c r="C26" s="60"/>
-      <c r="D26" s="59"/>
-      <c r="E26" s="61"/>
-      <c r="F26" s="61"/>
-      <c r="G26" s="61"/>
-      <c r="H26" s="61"/>
-    </row>
-    <row r="27" customFormat="false" ht="24.2" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A27" s="42" t="s">
-        <v>79</v>
-      </c>
-      <c r="B27" s="43" t="s">
-        <v>80</v>
-      </c>
-      <c r="C27" s="44" t="s">
-        <v>64</v>
-      </c>
-      <c r="D27" s="45" t="n">
-        <v>6</v>
-      </c>
-      <c r="E27" s="45"/>
-      <c r="F27" s="45"/>
-      <c r="G27" s="45"/>
-      <c r="H27" s="45"/>
+    <row r="27" customFormat="false" ht="11.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A27" s="57"/>
+      <c r="B27" s="58"/>
+      <c r="C27" s="59"/>
+      <c r="D27" s="58"/>
+      <c r="E27" s="60"/>
+      <c r="F27" s="60"/>
+      <c r="G27" s="60"/>
+      <c r="H27" s="60"/>
     </row>
     <row r="28" customFormat="false" ht="24.2" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A28" s="42" t="s">
-        <v>79</v>
+        <v>80</v>
       </c>
       <c r="B28" s="43" t="s">
-        <v>72</v>
-      </c>
-      <c r="C28" s="44" t="s">
         <v>81</v>
       </c>
-      <c r="D28" s="45" t="n">
+      <c r="C28" s="61" t="s">
+        <v>64</v>
+      </c>
+      <c r="D28" s="51" t="n">
+        <v>6</v>
+      </c>
+      <c r="E28" s="51"/>
+      <c r="F28" s="51"/>
+      <c r="G28" s="51"/>
+      <c r="H28" s="51"/>
+    </row>
+    <row r="29" customFormat="false" ht="24.2" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A29" s="42" t="s">
+        <v>80</v>
+      </c>
+      <c r="B29" s="43" t="s">
+        <v>73</v>
+      </c>
+      <c r="C29" s="61" t="s">
+        <v>82</v>
+      </c>
+      <c r="D29" s="51" t="n">
         <v>4</v>
       </c>
-      <c r="E28" s="45"/>
-      <c r="F28" s="45"/>
-      <c r="G28" s="45"/>
-      <c r="H28" s="45"/>
-    </row>
-    <row r="29" customFormat="false" ht="24.2" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A29" s="42"/>
-      <c r="B29" s="42"/>
-      <c r="C29" s="44" t="s">
-        <v>66</v>
-      </c>
-      <c r="D29" s="45" t="n">
-        <v>4</v>
-      </c>
-      <c r="E29" s="45"/>
-      <c r="F29" s="45"/>
-      <c r="G29" s="45"/>
-      <c r="H29" s="45"/>
+      <c r="E29" s="51"/>
+      <c r="F29" s="51"/>
+      <c r="G29" s="51"/>
+      <c r="H29" s="51"/>
     </row>
     <row r="30" customFormat="false" ht="24.2" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A30" s="42"/>
       <c r="B30" s="42"/>
-      <c r="C30" s="44" t="s">
+      <c r="C30" s="61" t="s">
+        <v>66</v>
+      </c>
+      <c r="D30" s="51" t="n">
+        <v>4</v>
+      </c>
+      <c r="E30" s="51"/>
+      <c r="F30" s="51"/>
+      <c r="G30" s="51"/>
+      <c r="H30" s="51"/>
+    </row>
+    <row r="31" customFormat="false" ht="24.2" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A31" s="42"/>
+      <c r="B31" s="42"/>
+      <c r="C31" s="61" t="s">
         <v>67</v>
       </c>
-      <c r="D30" s="45" t="n">
+      <c r="D31" s="51" t="n">
         <v>8</v>
       </c>
-      <c r="E30" s="45"/>
-      <c r="F30" s="45"/>
-      <c r="G30" s="45"/>
-      <c r="H30" s="45"/>
-    </row>
-    <row r="31" customFormat="false" ht="24.2" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A31" s="42" t="s">
-        <v>71</v>
-      </c>
-      <c r="B31" s="43" t="s">
+      <c r="E31" s="51"/>
+      <c r="F31" s="51"/>
+      <c r="G31" s="51"/>
+      <c r="H31" s="51"/>
+    </row>
+    <row r="32" customFormat="false" ht="24.2" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A32" s="42" t="s">
         <v>72</v>
       </c>
-      <c r="C31" s="51" t="s">
-        <v>82</v>
-      </c>
-      <c r="D31" s="45" t="n">
+      <c r="B32" s="43" t="s">
+        <v>73</v>
+      </c>
+      <c r="C32" s="62" t="s">
+        <v>83</v>
+      </c>
+      <c r="D32" s="51" t="n">
         <v>8</v>
       </c>
-      <c r="E31" s="45"/>
-      <c r="F31" s="45"/>
-      <c r="G31" s="45"/>
-      <c r="H31" s="45"/>
-    </row>
-    <row r="32" customFormat="false" ht="24.2" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A32" s="42"/>
-      <c r="B32" s="42"/>
-      <c r="C32" s="44" t="s">
-        <v>68</v>
-      </c>
-      <c r="D32" s="45" t="n">
-        <v>4</v>
-      </c>
-      <c r="E32" s="45"/>
-      <c r="F32" s="45"/>
-      <c r="G32" s="45"/>
-      <c r="H32" s="45"/>
+      <c r="E32" s="51"/>
+      <c r="F32" s="51"/>
+      <c r="G32" s="51"/>
+      <c r="H32" s="51"/>
     </row>
     <row r="33" customFormat="false" ht="24.2" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A33" s="42"/>
       <c r="B33" s="42"/>
-      <c r="C33" s="50" t="s">
-        <v>83</v>
-      </c>
-      <c r="D33" s="45" t="n">
-        <v>1</v>
-      </c>
-      <c r="E33" s="45"/>
-      <c r="F33" s="45"/>
-      <c r="G33" s="45"/>
-      <c r="H33" s="45"/>
-      <c r="I33" s="48"/>
-      <c r="J33" s="48"/>
+      <c r="C33" s="61" t="s">
+        <v>69</v>
+      </c>
+      <c r="D33" s="51" t="n">
+        <v>4</v>
+      </c>
+      <c r="E33" s="51"/>
+      <c r="F33" s="51"/>
+      <c r="G33" s="51"/>
+      <c r="H33" s="51"/>
     </row>
     <row r="34" customFormat="false" ht="24.2" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A34" s="42"/>
       <c r="B34" s="42"/>
-      <c r="C34" s="51" t="s">
+      <c r="C34" s="63" t="s">
         <v>84</v>
       </c>
-      <c r="D34" s="45" t="n">
+      <c r="D34" s="51" t="n">
         <v>1</v>
       </c>
-      <c r="E34" s="45"/>
-      <c r="F34" s="45"/>
-      <c r="G34" s="45"/>
-      <c r="H34" s="45"/>
+      <c r="E34" s="51"/>
+      <c r="F34" s="51"/>
+      <c r="G34" s="51"/>
+      <c r="H34" s="51"/>
+      <c r="I34" s="46"/>
+      <c r="J34" s="46"/>
     </row>
     <row r="35" customFormat="false" ht="24.2" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A35" s="42"/>
       <c r="B35" s="42"/>
-      <c r="C35" s="50" t="s">
+      <c r="C35" s="62" t="s">
         <v>85</v>
       </c>
-      <c r="D35" s="45" t="n">
-        <v>2</v>
-      </c>
-      <c r="E35" s="45"/>
-      <c r="F35" s="45"/>
-      <c r="G35" s="45"/>
-      <c r="H35" s="45"/>
+      <c r="D35" s="51" t="n">
+        <v>1</v>
+      </c>
+      <c r="E35" s="51"/>
+      <c r="F35" s="51"/>
+      <c r="G35" s="51"/>
+      <c r="H35" s="51"/>
     </row>
     <row r="36" customFormat="false" ht="24.2" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A36" s="42"/>
       <c r="B36" s="42"/>
-      <c r="C36" s="52" t="s">
-        <v>76</v>
-      </c>
-      <c r="D36" s="53" t="n">
-        <v>1</v>
-      </c>
-      <c r="E36" s="45"/>
-      <c r="F36" s="45"/>
-      <c r="G36" s="45"/>
-      <c r="H36" s="45"/>
+      <c r="C36" s="63" t="s">
+        <v>86</v>
+      </c>
+      <c r="D36" s="51" t="n">
+        <v>2</v>
+      </c>
+      <c r="E36" s="51"/>
+      <c r="F36" s="51"/>
+      <c r="G36" s="51"/>
+      <c r="H36" s="51"/>
     </row>
     <row r="37" customFormat="false" ht="24.2" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A37" s="42"/>
-      <c r="B37" s="54" t="s">
+      <c r="B37" s="42"/>
+      <c r="C37" s="52" t="s">
         <v>77</v>
       </c>
-      <c r="C37" s="54"/>
-      <c r="D37" s="54"/>
-      <c r="E37" s="62"/>
-      <c r="F37" s="62"/>
-      <c r="G37" s="62"/>
-      <c r="H37" s="62"/>
+      <c r="D37" s="48" t="n">
+        <v>1</v>
+      </c>
+      <c r="E37" s="51"/>
+      <c r="F37" s="51"/>
+      <c r="G37" s="51"/>
+      <c r="H37" s="51"/>
     </row>
     <row r="38" customFormat="false" ht="24.2" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A38" s="42"/>
-      <c r="B38" s="55" t="s">
+      <c r="B38" s="53" t="s">
         <v>78</v>
       </c>
-      <c r="C38" s="56" t="n">
-        <f aca="false">SUM(D27:D37)</f>
+      <c r="C38" s="53"/>
+      <c r="D38" s="53"/>
+      <c r="E38" s="64"/>
+      <c r="F38" s="64"/>
+      <c r="G38" s="64"/>
+      <c r="H38" s="64"/>
+    </row>
+    <row r="39" customFormat="false" ht="24.2" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A39" s="42"/>
+      <c r="B39" s="54" t="s">
+        <v>79</v>
+      </c>
+      <c r="C39" s="55" t="n">
+        <f aca="false">SUM(D28:D38)</f>
         <v>39</v>
       </c>
-      <c r="D38" s="55"/>
-      <c r="E38" s="63"/>
-      <c r="F38" s="63"/>
-      <c r="G38" s="63"/>
-      <c r="H38" s="63"/>
-      <c r="I38" s="32"/>
-      <c r="J38" s="32"/>
-    </row>
-    <row r="39" customFormat="false" ht="11.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A39" s="58"/>
-      <c r="B39" s="59"/>
-      <c r="C39" s="60"/>
-      <c r="D39" s="59"/>
-      <c r="E39" s="61"/>
-      <c r="F39" s="61"/>
-      <c r="G39" s="61"/>
-      <c r="H39" s="61"/>
-    </row>
-    <row r="40" customFormat="false" ht="25.35" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A40" s="42" t="s">
-        <v>79</v>
-      </c>
-      <c r="B40" s="43" t="s">
-        <v>86</v>
-      </c>
-      <c r="C40" s="44" t="s">
-        <v>64</v>
-      </c>
-      <c r="D40" s="45" t="n">
-        <v>6</v>
-      </c>
-      <c r="E40" s="45"/>
-      <c r="F40" s="45"/>
-      <c r="G40" s="45"/>
-      <c r="H40" s="45"/>
+      <c r="D39" s="54"/>
+      <c r="E39" s="65"/>
+      <c r="F39" s="65"/>
+      <c r="G39" s="65"/>
+      <c r="H39" s="65"/>
+      <c r="I39" s="32"/>
+      <c r="J39" s="32"/>
+    </row>
+    <row r="40" customFormat="false" ht="11.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A40" s="57"/>
+      <c r="B40" s="58"/>
+      <c r="C40" s="59"/>
+      <c r="D40" s="58"/>
+      <c r="E40" s="60"/>
+      <c r="F40" s="60"/>
+      <c r="G40" s="60"/>
+      <c r="H40" s="60"/>
     </row>
     <row r="41" customFormat="false" ht="25.35" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A41" s="42" t="s">
-        <v>79</v>
+        <v>80</v>
       </c>
       <c r="B41" s="43" t="s">
-        <v>72</v>
-      </c>
-      <c r="C41" s="44" t="s">
-        <v>81</v>
-      </c>
-      <c r="D41" s="45" t="n">
+        <v>87</v>
+      </c>
+      <c r="C41" s="61" t="s">
+        <v>64</v>
+      </c>
+      <c r="D41" s="51" t="n">
+        <v>6</v>
+      </c>
+      <c r="E41" s="51"/>
+      <c r="F41" s="51"/>
+      <c r="G41" s="51"/>
+      <c r="H41" s="51"/>
+    </row>
+    <row r="42" customFormat="false" ht="25.35" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A42" s="42" t="s">
+        <v>80</v>
+      </c>
+      <c r="B42" s="43" t="s">
+        <v>73</v>
+      </c>
+      <c r="C42" s="61" t="s">
+        <v>82</v>
+      </c>
+      <c r="D42" s="51" t="n">
         <v>4</v>
       </c>
-      <c r="E41" s="45"/>
-      <c r="F41" s="45"/>
-      <c r="G41" s="45"/>
-      <c r="H41" s="45"/>
-    </row>
-    <row r="42" customFormat="false" ht="25.35" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A42" s="42"/>
-      <c r="B42" s="42"/>
-      <c r="C42" s="44" t="s">
-        <v>66</v>
-      </c>
-      <c r="D42" s="45" t="n">
-        <v>4</v>
-      </c>
-      <c r="E42" s="45"/>
-      <c r="F42" s="45"/>
-      <c r="G42" s="45"/>
-      <c r="H42" s="45"/>
+      <c r="E42" s="51"/>
+      <c r="F42" s="51"/>
+      <c r="G42" s="51"/>
+      <c r="H42" s="51"/>
     </row>
     <row r="43" customFormat="false" ht="25.35" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A43" s="42"/>
       <c r="B43" s="42"/>
-      <c r="C43" s="44" t="s">
+      <c r="C43" s="61" t="s">
+        <v>66</v>
+      </c>
+      <c r="D43" s="51" t="n">
+        <v>4</v>
+      </c>
+      <c r="E43" s="51"/>
+      <c r="F43" s="51"/>
+      <c r="G43" s="51"/>
+      <c r="H43" s="51"/>
+    </row>
+    <row r="44" customFormat="false" ht="25.35" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A44" s="42"/>
+      <c r="B44" s="42"/>
+      <c r="C44" s="61" t="s">
         <v>67</v>
       </c>
-      <c r="D43" s="45" t="n">
+      <c r="D44" s="51" t="n">
         <v>8</v>
       </c>
-      <c r="E43" s="45"/>
-      <c r="F43" s="45"/>
-      <c r="G43" s="45"/>
-      <c r="H43" s="45"/>
-    </row>
-    <row r="44" customFormat="false" ht="25.35" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A44" s="42" t="s">
-        <v>71</v>
-      </c>
-      <c r="B44" s="43" t="s">
+      <c r="E44" s="51"/>
+      <c r="F44" s="51"/>
+      <c r="G44" s="51"/>
+      <c r="H44" s="51"/>
+    </row>
+    <row r="45" customFormat="false" ht="25.35" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A45" s="42" t="s">
         <v>72</v>
       </c>
-      <c r="C44" s="51" t="s">
-        <v>82</v>
-      </c>
-      <c r="D44" s="45" t="n">
+      <c r="B45" s="43" t="s">
+        <v>73</v>
+      </c>
+      <c r="C45" s="62" t="s">
+        <v>88</v>
+      </c>
+      <c r="D45" s="51" t="n">
         <v>8</v>
       </c>
-      <c r="E44" s="45"/>
-      <c r="F44" s="45"/>
-      <c r="G44" s="45"/>
-      <c r="H44" s="45"/>
-    </row>
-    <row r="45" customFormat="false" ht="25.35" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A45" s="42"/>
-      <c r="B45" s="42"/>
-      <c r="C45" s="44" t="s">
-        <v>68</v>
-      </c>
-      <c r="D45" s="45" t="n">
-        <v>4</v>
-      </c>
-      <c r="E45" s="45"/>
-      <c r="F45" s="45"/>
-      <c r="G45" s="45"/>
-      <c r="H45" s="45"/>
+      <c r="E45" s="51"/>
+      <c r="F45" s="51"/>
+      <c r="G45" s="51"/>
+      <c r="H45" s="51"/>
     </row>
     <row r="46" customFormat="false" ht="25.35" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A46" s="42"/>
       <c r="B46" s="42"/>
-      <c r="C46" s="50" t="s">
-        <v>83</v>
-      </c>
-      <c r="D46" s="45" t="n">
-        <v>1</v>
-      </c>
-      <c r="E46" s="45"/>
-      <c r="F46" s="45"/>
-      <c r="G46" s="45"/>
-      <c r="H46" s="45"/>
+      <c r="C46" s="61" t="s">
+        <v>69</v>
+      </c>
+      <c r="D46" s="51" t="n">
+        <v>4</v>
+      </c>
+      <c r="E46" s="51"/>
+      <c r="F46" s="51"/>
+      <c r="G46" s="51"/>
+      <c r="H46" s="51"/>
     </row>
     <row r="47" customFormat="false" ht="25.35" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A47" s="42"/>
       <c r="B47" s="42"/>
-      <c r="C47" s="51" t="s">
+      <c r="C47" s="63" t="s">
         <v>84</v>
       </c>
-      <c r="D47" s="45" t="n">
+      <c r="D47" s="51" t="n">
         <v>1</v>
       </c>
-      <c r="E47" s="45"/>
-      <c r="F47" s="45"/>
-      <c r="G47" s="45"/>
-      <c r="H47" s="45"/>
+      <c r="E47" s="51"/>
+      <c r="F47" s="51"/>
+      <c r="G47" s="51"/>
+      <c r="H47" s="51"/>
     </row>
     <row r="48" customFormat="false" ht="25.35" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A48" s="42"/>
       <c r="B48" s="42"/>
-      <c r="C48" s="50" t="s">
+      <c r="C48" s="62" t="s">
         <v>85</v>
       </c>
-      <c r="D48" s="45" t="n">
-        <v>2</v>
-      </c>
-      <c r="E48" s="45"/>
-      <c r="F48" s="45"/>
-      <c r="G48" s="45"/>
-      <c r="H48" s="45"/>
+      <c r="D48" s="51" t="n">
+        <v>1</v>
+      </c>
+      <c r="E48" s="51"/>
+      <c r="F48" s="51"/>
+      <c r="G48" s="51"/>
+      <c r="H48" s="51"/>
     </row>
     <row r="49" customFormat="false" ht="25.35" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A49" s="42"/>
       <c r="B49" s="42"/>
-      <c r="C49" s="52" t="s">
-        <v>76</v>
-      </c>
-      <c r="D49" s="53" t="n">
-        <v>1</v>
-      </c>
-      <c r="E49" s="45"/>
-      <c r="F49" s="45"/>
-      <c r="G49" s="45"/>
-      <c r="H49" s="45"/>
+      <c r="C49" s="63" t="s">
+        <v>86</v>
+      </c>
+      <c r="D49" s="51" t="n">
+        <v>2</v>
+      </c>
+      <c r="E49" s="51"/>
+      <c r="F49" s="51"/>
+      <c r="G49" s="51"/>
+      <c r="H49" s="51"/>
     </row>
     <row r="50" customFormat="false" ht="25.35" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A50" s="42"/>
-      <c r="B50" s="54" t="s">
+      <c r="B50" s="42"/>
+      <c r="C50" s="52" t="s">
         <v>77</v>
       </c>
-      <c r="C50" s="54"/>
-      <c r="D50" s="54"/>
-      <c r="E50" s="54"/>
-      <c r="F50" s="54"/>
-      <c r="G50" s="54"/>
-      <c r="H50" s="54"/>
+      <c r="D50" s="48" t="n">
+        <v>1</v>
+      </c>
+      <c r="E50" s="51"/>
+      <c r="F50" s="51"/>
+      <c r="G50" s="51"/>
+      <c r="H50" s="51"/>
     </row>
     <row r="51" customFormat="false" ht="25.35" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A51" s="42"/>
-      <c r="B51" s="55" t="s">
+      <c r="B51" s="53" t="s">
         <v>78</v>
       </c>
-      <c r="C51" s="56" t="n">
-        <f aca="false">SUM(D40:D50)</f>
+      <c r="C51" s="53"/>
+      <c r="D51" s="53"/>
+      <c r="E51" s="53"/>
+      <c r="F51" s="53"/>
+      <c r="G51" s="53"/>
+      <c r="H51" s="53"/>
+    </row>
+    <row r="52" customFormat="false" ht="25.35" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A52" s="42"/>
+      <c r="B52" s="54" t="s">
+        <v>79</v>
+      </c>
+      <c r="C52" s="55" t="n">
+        <f aca="false">SUM(D41:D51)</f>
         <v>39</v>
       </c>
-      <c r="D51" s="55"/>
-      <c r="E51" s="55"/>
-      <c r="F51" s="55"/>
-      <c r="G51" s="55"/>
-      <c r="H51" s="55"/>
-    </row>
-    <row r="52" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A52" s="64"/>
-      <c r="B52" s="65"/>
-      <c r="C52" s="66"/>
-      <c r="D52" s="67"/>
-      <c r="E52" s="67"/>
-      <c r="F52" s="67"/>
-      <c r="G52" s="67"/>
-      <c r="H52" s="68"/>
+      <c r="D52" s="54"/>
+      <c r="E52" s="54"/>
+      <c r="F52" s="54"/>
+      <c r="G52" s="54"/>
+      <c r="H52" s="54"/>
+    </row>
+    <row r="53" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A53" s="66"/>
+      <c r="B53" s="67"/>
+      <c r="C53" s="68"/>
+      <c r="D53" s="69"/>
+      <c r="E53" s="69"/>
+      <c r="F53" s="69"/>
+      <c r="G53" s="69"/>
+      <c r="H53" s="70"/>
     </row>
   </sheetData>
   <mergeCells count="10">
@@ -5358,12 +5565,12 @@
     <mergeCell ref="A7:A10"/>
     <mergeCell ref="B7:B10"/>
     <mergeCell ref="D7:H7"/>
-    <mergeCell ref="A11:A25"/>
-    <mergeCell ref="B11:B23"/>
-    <mergeCell ref="A27:A38"/>
-    <mergeCell ref="B27:B36"/>
-    <mergeCell ref="A40:A51"/>
-    <mergeCell ref="B40:B49"/>
+    <mergeCell ref="A11:A26"/>
+    <mergeCell ref="B11:B24"/>
+    <mergeCell ref="A28:A39"/>
+    <mergeCell ref="B28:B37"/>
+    <mergeCell ref="A41:A52"/>
+    <mergeCell ref="B41:B50"/>
   </mergeCells>
   <printOptions headings="false" gridLines="true" gridLinesSet="true" horizontalCentered="true" verticalCentered="false"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>
@@ -5382,105 +5589,105 @@
   </sheetPr>
   <dimension ref="A1:F10"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="75" zoomScaleNormal="75" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A4" colorId="64" zoomScale="75" zoomScaleNormal="75" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="I11" activeCellId="0" sqref="I11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="69" width="23.51"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="2" style="69" width="13.68"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="71" width="23.51"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="2" style="71" width="13.68"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="18" min="7" style="0" width="13.68"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="19" style="69" width="14.43"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="19" style="71" width="14.43"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="26.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A1" s="70"/>
-      <c r="B1" s="71"/>
-      <c r="C1" s="72"/>
-      <c r="D1" s="72"/>
-      <c r="E1" s="72"/>
-      <c r="F1" s="73" t="s">
-        <v>87</v>
+      <c r="A1" s="72"/>
+      <c r="B1" s="73"/>
+      <c r="C1" s="74"/>
+      <c r="D1" s="74"/>
+      <c r="E1" s="74"/>
+      <c r="F1" s="75" t="s">
+        <v>89</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="26.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B2" s="71"/>
-      <c r="C2" s="72"/>
-      <c r="D2" s="72"/>
-      <c r="E2" s="72"/>
-      <c r="F2" s="74"/>
+      <c r="B2" s="73"/>
+      <c r="C2" s="74"/>
+      <c r="D2" s="74"/>
+      <c r="E2" s="74"/>
+      <c r="F2" s="76"/>
     </row>
     <row r="3" customFormat="false" ht="26.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B3" s="71"/>
-      <c r="C3" s="72"/>
-      <c r="D3" s="72"/>
-      <c r="E3" s="72"/>
-      <c r="F3" s="74"/>
+      <c r="B3" s="73"/>
+      <c r="C3" s="74"/>
+      <c r="D3" s="74"/>
+      <c r="E3" s="74"/>
+      <c r="F3" s="76"/>
     </row>
     <row r="4" customFormat="false" ht="26.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B4" s="71"/>
-      <c r="C4" s="75"/>
-      <c r="D4" s="72"/>
-      <c r="E4" s="72"/>
-      <c r="F4" s="74"/>
+      <c r="B4" s="73"/>
+      <c r="C4" s="77"/>
+      <c r="D4" s="74"/>
+      <c r="E4" s="74"/>
+      <c r="F4" s="76"/>
     </row>
     <row r="5" customFormat="false" ht="26.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
     <row r="6" customFormat="false" ht="26.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
     <row r="7" customFormat="false" ht="26.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A7" s="76" t="s">
+      <c r="A7" s="78" t="s">
         <v>54</v>
       </c>
-      <c r="B7" s="77" t="s">
+      <c r="B7" s="79" t="s">
         <v>55</v>
       </c>
-      <c r="C7" s="77" t="s">
-        <v>88</v>
-      </c>
-      <c r="D7" s="77" t="s">
-        <v>89</v>
-      </c>
-      <c r="E7" s="77" t="s">
+      <c r="C7" s="79" t="s">
         <v>90</v>
       </c>
-      <c r="F7" s="77" t="s">
+      <c r="D7" s="79" t="s">
         <v>91</v>
       </c>
+      <c r="E7" s="79" t="s">
+        <v>92</v>
+      </c>
+      <c r="F7" s="79" t="s">
+        <v>93</v>
+      </c>
     </row>
     <row r="8" customFormat="false" ht="26.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A8" s="76" t="s">
+      <c r="A8" s="78" t="s">
         <v>58</v>
       </c>
-      <c r="B8" s="78" t="n">
+      <c r="B8" s="80" t="n">
         <f aca="false">SUM(B10:B18,B22:B23)</f>
         <v>0</v>
       </c>
-      <c r="C8" s="78" t="n">
+      <c r="C8" s="80" t="n">
         <f aca="false">SUM(C10:C18)</f>
         <v>0</v>
       </c>
-      <c r="D8" s="78" t="n">
+      <c r="D8" s="80" t="n">
         <f aca="false">SUM(D10:D18)</f>
         <v>0</v>
       </c>
-      <c r="E8" s="78" t="n">
+      <c r="E8" s="80" t="n">
         <f aca="false">SUM(E10:E18)</f>
         <v>0</v>
       </c>
-      <c r="F8" s="78" t="n">
+      <c r="F8" s="80" t="n">
         <f aca="false">SUM(F10:F18)</f>
         <v>0</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="26.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A9" s="76" t="s">
+      <c r="A9" s="78" t="s">
         <v>59</v>
       </c>
-      <c r="B9" s="78"/>
-      <c r="C9" s="78"/>
-      <c r="D9" s="78"/>
-      <c r="E9" s="78"/>
-      <c r="F9" s="78" t="e">
+      <c r="B9" s="80"/>
+      <c r="C9" s="80"/>
+      <c r="D9" s="80"/>
+      <c r="E9" s="80"/>
+      <c r="F9" s="80" t="e">
         <f aca="false">SUM(#REF!)</f>
         <v>#REF!</v>
       </c>
@@ -5523,10 +5730,10 @@
   </sheetPr>
   <dimension ref="A1:AMJ25"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A4" colorId="64" zoomScale="75" zoomScaleNormal="75" zoomScalePageLayoutView="100" workbookViewId="0">
-      <pane xSplit="3" ySplit="0" topLeftCell="D4" activePane="topRight" state="frozen"/>
-      <selection pane="topLeft" activeCell="A4" activeCellId="0" sqref="A4"/>
-      <selection pane="topRight" activeCell="A11" activeCellId="0" sqref="A11"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A7" colorId="64" zoomScale="75" zoomScaleNormal="75" zoomScalePageLayoutView="100" workbookViewId="0">
+      <pane xSplit="3" ySplit="0" topLeftCell="E7" activePane="topRight" state="frozen"/>
+      <selection pane="topLeft" activeCell="A7" activeCellId="0" sqref="A7"/>
+      <selection pane="topRight" activeCell="E1" activeCellId="0" sqref="E1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -5622,11 +5829,11 @@
       <c r="F7" s="37"/>
       <c r="G7" s="37"/>
       <c r="H7" s="37"/>
-      <c r="I7" s="79"/>
-      <c r="Q7" s="80"/>
-      <c r="R7" s="81"/>
-      <c r="S7" s="81"/>
-      <c r="T7" s="82"/>
+      <c r="I7" s="81"/>
+      <c r="Q7" s="82"/>
+      <c r="R7" s="83"/>
+      <c r="S7" s="83"/>
+      <c r="T7" s="84"/>
     </row>
     <row r="8" customFormat="false" ht="20.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A8" s="36"/>
@@ -5638,21 +5845,21 @@
         <v>55</v>
       </c>
       <c r="E8" s="40" t="s">
-        <v>88</v>
+        <v>90</v>
       </c>
       <c r="F8" s="40" t="s">
-        <v>89</v>
+        <v>91</v>
       </c>
       <c r="G8" s="40" t="s">
-        <v>90</v>
+        <v>92</v>
       </c>
       <c r="H8" s="40" t="s">
-        <v>91</v>
-      </c>
-      <c r="Q8" s="80"/>
-      <c r="R8" s="81"/>
-      <c r="S8" s="81"/>
-      <c r="T8" s="83"/>
+        <v>93</v>
+      </c>
+      <c r="Q8" s="82"/>
+      <c r="R8" s="83"/>
+      <c r="S8" s="83"/>
+      <c r="T8" s="85"/>
     </row>
     <row r="9" customFormat="false" ht="20.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A9" s="36"/>
@@ -5680,8 +5887,8 @@
         <f aca="false">SUM(H11:H24)</f>
         <v>0</v>
       </c>
-      <c r="Q9" s="84"/>
-      <c r="T9" s="83"/>
+      <c r="Q9" s="86"/>
+      <c r="T9" s="85"/>
     </row>
     <row r="10" customFormat="false" ht="20.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A10" s="36"/>
@@ -5697,30 +5904,30 @@
         <f aca="false">SUM(#REF!)</f>
         <v>#REF!</v>
       </c>
-      <c r="Q10" s="84"/>
-      <c r="T10" s="83"/>
+      <c r="Q10" s="86"/>
+      <c r="T10" s="85"/>
     </row>
     <row r="11" s="1" customFormat="true" ht="27.65" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A11" s="42" t="s">
         <v>60</v>
       </c>
-      <c r="B11" s="85" t="s">
-        <v>92</v>
-      </c>
-      <c r="C11" s="44" t="s">
+      <c r="B11" s="87" t="s">
+        <v>94</v>
+      </c>
+      <c r="C11" s="61" t="s">
         <v>62</v>
       </c>
-      <c r="D11" s="45" t="n">
+      <c r="D11" s="51" t="n">
         <v>4</v>
       </c>
-      <c r="E11" s="45" t="n">
+      <c r="E11" s="51" t="n">
         <v>0</v>
       </c>
-      <c r="F11" s="45"/>
-      <c r="G11" s="45"/>
-      <c r="H11" s="45"/>
-      <c r="Q11" s="86"/>
-      <c r="T11" s="87"/>
+      <c r="F11" s="51"/>
+      <c r="G11" s="51"/>
+      <c r="H11" s="51"/>
+      <c r="Q11" s="88"/>
+      <c r="T11" s="89"/>
       <c r="AMF11" s="0"/>
       <c r="AMG11" s="0"/>
       <c r="AMH11" s="0"/>
@@ -5730,20 +5937,20 @@
     <row r="12" s="1" customFormat="true" ht="27.65" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A12" s="42"/>
       <c r="B12" s="42"/>
-      <c r="C12" s="44" t="s">
+      <c r="C12" s="61" t="s">
         <v>63</v>
       </c>
-      <c r="D12" s="45" t="n">
+      <c r="D12" s="51" t="n">
         <v>8</v>
       </c>
-      <c r="E12" s="45" t="n">
+      <c r="E12" s="51" t="n">
         <v>6</v>
       </c>
-      <c r="F12" s="45"/>
-      <c r="G12" s="45"/>
-      <c r="H12" s="45"/>
-      <c r="Q12" s="86"/>
-      <c r="T12" s="87"/>
+      <c r="F12" s="51"/>
+      <c r="G12" s="51"/>
+      <c r="H12" s="51"/>
+      <c r="Q12" s="88"/>
+      <c r="T12" s="89"/>
       <c r="AMF12" s="0"/>
       <c r="AMG12" s="0"/>
       <c r="AMH12" s="0"/>
@@ -5753,20 +5960,20 @@
     <row r="13" s="1" customFormat="true" ht="27.65" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A13" s="42"/>
       <c r="B13" s="42"/>
-      <c r="C13" s="44" t="s">
+      <c r="C13" s="61" t="s">
         <v>64</v>
       </c>
-      <c r="D13" s="45" t="n">
+      <c r="D13" s="51" t="n">
         <v>6</v>
       </c>
-      <c r="E13" s="45" t="n">
+      <c r="E13" s="51" t="n">
         <v>4</v>
       </c>
-      <c r="F13" s="45"/>
-      <c r="G13" s="45"/>
-      <c r="H13" s="45"/>
-      <c r="Q13" s="86"/>
-      <c r="T13" s="87"/>
+      <c r="F13" s="51"/>
+      <c r="G13" s="51"/>
+      <c r="H13" s="51"/>
+      <c r="Q13" s="88"/>
+      <c r="T13" s="89"/>
       <c r="AMF13" s="0"/>
       <c r="AMG13" s="0"/>
       <c r="AMH13" s="0"/>
@@ -5775,19 +5982,19 @@
     </row>
     <row r="14" s="1" customFormat="true" ht="27.65" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A14" s="42"/>
-      <c r="B14" s="85"/>
-      <c r="C14" s="44" t="s">
+      <c r="B14" s="87"/>
+      <c r="C14" s="61" t="s">
         <v>65</v>
       </c>
-      <c r="D14" s="45" t="n">
+      <c r="D14" s="51" t="n">
         <v>4</v>
       </c>
-      <c r="E14" s="45"/>
-      <c r="F14" s="45"/>
-      <c r="G14" s="45"/>
-      <c r="H14" s="45"/>
-      <c r="Q14" s="86"/>
-      <c r="T14" s="87"/>
+      <c r="E14" s="51"/>
+      <c r="F14" s="51"/>
+      <c r="G14" s="51"/>
+      <c r="H14" s="51"/>
+      <c r="Q14" s="88"/>
+      <c r="T14" s="89"/>
       <c r="AMF14" s="0"/>
       <c r="AMG14" s="0"/>
       <c r="AMH14" s="0"/>
@@ -5797,18 +6004,18 @@
     <row r="15" s="1" customFormat="true" ht="27.65" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A15" s="42"/>
       <c r="B15" s="42"/>
-      <c r="C15" s="44" t="s">
+      <c r="C15" s="61" t="s">
         <v>66</v>
       </c>
-      <c r="D15" s="45" t="n">
+      <c r="D15" s="51" t="n">
         <v>4</v>
       </c>
-      <c r="E15" s="45"/>
-      <c r="F15" s="45"/>
-      <c r="G15" s="45"/>
-      <c r="H15" s="45"/>
-      <c r="Q15" s="86"/>
-      <c r="T15" s="87"/>
+      <c r="E15" s="51"/>
+      <c r="F15" s="51"/>
+      <c r="G15" s="51"/>
+      <c r="H15" s="51"/>
+      <c r="Q15" s="88"/>
+      <c r="T15" s="89"/>
       <c r="AMF15" s="0"/>
       <c r="AMG15" s="0"/>
       <c r="AMH15" s="0"/>
@@ -5818,18 +6025,18 @@
     <row r="16" s="1" customFormat="true" ht="27.65" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A16" s="42"/>
       <c r="B16" s="42"/>
-      <c r="C16" s="44" t="s">
+      <c r="C16" s="61" t="s">
         <v>67</v>
       </c>
-      <c r="D16" s="45" t="n">
+      <c r="D16" s="51" t="n">
         <v>8</v>
       </c>
-      <c r="E16" s="45"/>
-      <c r="F16" s="45"/>
-      <c r="G16" s="45"/>
-      <c r="H16" s="45"/>
-      <c r="Q16" s="86"/>
-      <c r="T16" s="87"/>
+      <c r="E16" s="51"/>
+      <c r="F16" s="51"/>
+      <c r="G16" s="51"/>
+      <c r="H16" s="51"/>
+      <c r="Q16" s="88"/>
+      <c r="T16" s="89"/>
       <c r="AMF16" s="0"/>
       <c r="AMG16" s="0"/>
       <c r="AMH16" s="0"/>
@@ -5838,23 +6045,23 @@
     </row>
     <row r="17" s="1" customFormat="true" ht="27.65" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A17" s="42" t="s">
-        <v>71</v>
-      </c>
-      <c r="B17" s="85" t="s">
         <v>72</v>
       </c>
-      <c r="C17" s="51" t="s">
-        <v>82</v>
-      </c>
-      <c r="D17" s="45" t="n">
+      <c r="B17" s="87" t="s">
+        <v>73</v>
+      </c>
+      <c r="C17" s="62" t="s">
+        <v>95</v>
+      </c>
+      <c r="D17" s="51" t="n">
         <v>8</v>
       </c>
-      <c r="E17" s="45"/>
-      <c r="F17" s="45"/>
-      <c r="G17" s="45"/>
-      <c r="H17" s="45"/>
-      <c r="Q17" s="86"/>
-      <c r="T17" s="87"/>
+      <c r="E17" s="51"/>
+      <c r="F17" s="51"/>
+      <c r="G17" s="51"/>
+      <c r="H17" s="51"/>
+      <c r="Q17" s="88"/>
+      <c r="T17" s="89"/>
       <c r="AMF17" s="0"/>
       <c r="AMG17" s="0"/>
       <c r="AMH17" s="0"/>
@@ -5864,18 +6071,18 @@
     <row r="18" s="1" customFormat="true" ht="27.65" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A18" s="42"/>
       <c r="B18" s="42"/>
-      <c r="C18" s="44" t="s">
-        <v>68</v>
-      </c>
-      <c r="D18" s="45" t="n">
+      <c r="C18" s="61" t="s">
+        <v>69</v>
+      </c>
+      <c r="D18" s="51" t="n">
         <v>4</v>
       </c>
-      <c r="E18" s="45"/>
-      <c r="F18" s="45"/>
-      <c r="G18" s="45"/>
-      <c r="H18" s="45"/>
-      <c r="Q18" s="86"/>
-      <c r="T18" s="87"/>
+      <c r="E18" s="51"/>
+      <c r="F18" s="51"/>
+      <c r="G18" s="51"/>
+      <c r="H18" s="51"/>
+      <c r="Q18" s="88"/>
+      <c r="T18" s="89"/>
       <c r="AMF18" s="0"/>
       <c r="AMG18" s="0"/>
       <c r="AMH18" s="0"/>
@@ -5885,18 +6092,18 @@
     <row r="19" s="1" customFormat="true" ht="27.65" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A19" s="42"/>
       <c r="B19" s="42"/>
-      <c r="C19" s="50" t="s">
-        <v>83</v>
-      </c>
-      <c r="D19" s="45" t="n">
+      <c r="C19" s="63" t="s">
+        <v>84</v>
+      </c>
+      <c r="D19" s="51" t="n">
         <v>1</v>
       </c>
-      <c r="E19" s="45"/>
-      <c r="F19" s="45"/>
-      <c r="G19" s="45"/>
-      <c r="H19" s="45"/>
-      <c r="Q19" s="86"/>
-      <c r="T19" s="87"/>
+      <c r="E19" s="51"/>
+      <c r="F19" s="51"/>
+      <c r="G19" s="51"/>
+      <c r="H19" s="51"/>
+      <c r="Q19" s="88"/>
+      <c r="T19" s="89"/>
       <c r="AMF19" s="0"/>
       <c r="AMG19" s="0"/>
       <c r="AMH19" s="0"/>
@@ -5906,18 +6113,18 @@
     <row r="20" s="1" customFormat="true" ht="27.65" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A20" s="42"/>
       <c r="B20" s="42"/>
-      <c r="C20" s="51" t="s">
-        <v>84</v>
-      </c>
-      <c r="D20" s="45" t="n">
+      <c r="C20" s="62" t="s">
+        <v>85</v>
+      </c>
+      <c r="D20" s="51" t="n">
         <v>1</v>
       </c>
-      <c r="E20" s="45"/>
-      <c r="F20" s="45"/>
-      <c r="G20" s="45"/>
-      <c r="H20" s="45"/>
-      <c r="Q20" s="86"/>
-      <c r="T20" s="87"/>
+      <c r="E20" s="51"/>
+      <c r="F20" s="51"/>
+      <c r="G20" s="51"/>
+      <c r="H20" s="51"/>
+      <c r="Q20" s="88"/>
+      <c r="T20" s="89"/>
       <c r="AMF20" s="0"/>
       <c r="AMG20" s="0"/>
       <c r="AMH20" s="0"/>
@@ -5927,18 +6134,18 @@
     <row r="21" s="1" customFormat="true" ht="27.65" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A21" s="42"/>
       <c r="B21" s="42"/>
-      <c r="C21" s="50" t="s">
-        <v>85</v>
-      </c>
-      <c r="D21" s="45" t="n">
+      <c r="C21" s="63" t="s">
+        <v>86</v>
+      </c>
+      <c r="D21" s="51" t="n">
         <v>2</v>
       </c>
-      <c r="E21" s="45"/>
-      <c r="F21" s="45"/>
-      <c r="G21" s="45"/>
-      <c r="H21" s="45"/>
-      <c r="Q21" s="86"/>
-      <c r="T21" s="87"/>
+      <c r="E21" s="51"/>
+      <c r="F21" s="51"/>
+      <c r="G21" s="51"/>
+      <c r="H21" s="51"/>
+      <c r="Q21" s="88"/>
+      <c r="T21" s="89"/>
       <c r="AMF21" s="0"/>
       <c r="AMG21" s="0"/>
       <c r="AMH21" s="0"/>
@@ -5949,17 +6156,17 @@
       <c r="A22" s="42"/>
       <c r="B22" s="42"/>
       <c r="C22" s="52" t="s">
-        <v>76</v>
-      </c>
-      <c r="D22" s="53" t="n">
+        <v>77</v>
+      </c>
+      <c r="D22" s="48" t="n">
         <v>1</v>
       </c>
-      <c r="E22" s="45"/>
-      <c r="F22" s="45"/>
-      <c r="G22" s="45"/>
-      <c r="H22" s="45"/>
-      <c r="Q22" s="86"/>
-      <c r="T22" s="87"/>
+      <c r="E22" s="51"/>
+      <c r="F22" s="51"/>
+      <c r="G22" s="51"/>
+      <c r="H22" s="51"/>
+      <c r="Q22" s="88"/>
+      <c r="T22" s="89"/>
       <c r="AMF22" s="0"/>
       <c r="AMG22" s="0"/>
       <c r="AMH22" s="0"/>
@@ -5968,17 +6175,17 @@
     </row>
     <row r="23" s="1" customFormat="true" ht="34.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A23" s="42"/>
-      <c r="B23" s="54" t="s">
-        <v>77</v>
-      </c>
-      <c r="C23" s="54"/>
-      <c r="D23" s="54"/>
-      <c r="E23" s="54"/>
-      <c r="F23" s="54"/>
-      <c r="G23" s="54"/>
-      <c r="H23" s="54"/>
-      <c r="Q23" s="86"/>
-      <c r="T23" s="87"/>
+      <c r="B23" s="53" t="s">
+        <v>78</v>
+      </c>
+      <c r="C23" s="53"/>
+      <c r="D23" s="53"/>
+      <c r="E23" s="53"/>
+      <c r="F23" s="53"/>
+      <c r="G23" s="53"/>
+      <c r="H23" s="53"/>
+      <c r="Q23" s="88"/>
+      <c r="T23" s="89"/>
       <c r="AMF23" s="0"/>
       <c r="AMG23" s="0"/>
       <c r="AMH23" s="0"/>
@@ -5987,24 +6194,24 @@
     </row>
     <row r="24" s="1" customFormat="true" ht="34.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A24" s="42"/>
-      <c r="B24" s="55" t="s">
-        <v>78</v>
-      </c>
-      <c r="C24" s="56" t="n">
+      <c r="B24" s="54" t="s">
+        <v>79</v>
+      </c>
+      <c r="C24" s="55" t="n">
         <f aca="false">SUM(D11:D23)</f>
         <v>51</v>
       </c>
-      <c r="D24" s="55"/>
-      <c r="E24" s="55"/>
-      <c r="F24" s="55"/>
-      <c r="G24" s="55"/>
-      <c r="H24" s="55"/>
-      <c r="I24" s="48"/>
-      <c r="J24" s="48"/>
-      <c r="Q24" s="88"/>
-      <c r="R24" s="89"/>
-      <c r="S24" s="89"/>
-      <c r="T24" s="90"/>
+      <c r="D24" s="54"/>
+      <c r="E24" s="54"/>
+      <c r="F24" s="54"/>
+      <c r="G24" s="54"/>
+      <c r="H24" s="54"/>
+      <c r="I24" s="46"/>
+      <c r="J24" s="46"/>
+      <c r="Q24" s="90"/>
+      <c r="R24" s="91"/>
+      <c r="S24" s="91"/>
+      <c r="T24" s="92"/>
       <c r="AMF24" s="0"/>
       <c r="AMG24" s="0"/>
       <c r="AMH24" s="0"/>
@@ -6012,14 +6219,14 @@
       <c r="AMJ24" s="0"/>
     </row>
     <row r="25" s="1" customFormat="true" ht="8.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A25" s="64"/>
-      <c r="B25" s="65"/>
-      <c r="C25" s="66"/>
-      <c r="D25" s="67"/>
-      <c r="E25" s="67"/>
-      <c r="F25" s="67"/>
-      <c r="G25" s="67"/>
-      <c r="H25" s="68"/>
+      <c r="A25" s="66"/>
+      <c r="B25" s="67"/>
+      <c r="C25" s="68"/>
+      <c r="D25" s="69"/>
+      <c r="E25" s="69"/>
+      <c r="F25" s="69"/>
+      <c r="G25" s="69"/>
+      <c r="H25" s="70"/>
       <c r="AMF25" s="0"/>
       <c r="AMG25" s="0"/>
       <c r="AMH25" s="0"/>
@@ -6054,15 +6261,15 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:AMJ1048576"/>
+  <dimension ref="A1:O23"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="75" zoomScaleNormal="75" zoomScalePageLayoutView="100" workbookViewId="0">
-      <pane xSplit="2" ySplit="0" topLeftCell="C1" activePane="topRight" state="frozen"/>
-      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-      <selection pane="topRight" activeCell="A11" activeCellId="0" sqref="A11"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A13" colorId="64" zoomScale="75" zoomScaleNormal="75" zoomScalePageLayoutView="100" workbookViewId="0">
+      <pane xSplit="2" ySplit="0" topLeftCell="I13" activePane="topRight" state="frozen"/>
+      <selection pane="topLeft" activeCell="A13" activeCellId="0" sqref="A13"/>
+      <selection pane="topRight" activeCell="C22" activeCellId="0" sqref="C22"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="20.98"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="46.68"/>
@@ -6074,11 +6281,16 @@
       <c r="A1" s="3"/>
       <c r="B1" s="4"/>
       <c r="C1" s="5"/>
-      <c r="D1" s="6"/>
-      <c r="E1" s="7"/>
-      <c r="F1" s="7"/>
-      <c r="G1" s="7"/>
-      <c r="H1" s="7"/>
+      <c r="D1" s="5"/>
+      <c r="E1" s="6"/>
+      <c r="F1" s="6"/>
+      <c r="G1" s="6"/>
+      <c r="H1" s="6"/>
+      <c r="I1" s="6"/>
+      <c r="J1" s="7"/>
+      <c r="K1" s="7"/>
+      <c r="L1" s="7"/>
+      <c r="M1" s="7"/>
     </row>
     <row r="2" customFormat="false" ht="29.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="9" t="s">
@@ -6091,6 +6303,11 @@
       <c r="F2" s="9"/>
       <c r="G2" s="9"/>
       <c r="H2" s="9"/>
+      <c r="I2" s="9"/>
+      <c r="J2" s="9"/>
+      <c r="K2" s="9"/>
+      <c r="L2" s="9"/>
+      <c r="M2" s="9"/>
     </row>
     <row r="3" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="10"/>
@@ -6098,11 +6315,16 @@
       <c r="C3" s="10" t="s">
         <v>1</v>
       </c>
-      <c r="D3" s="11"/>
+      <c r="D3" s="10"/>
       <c r="E3" s="11"/>
       <c r="F3" s="11"/>
       <c r="G3" s="11"/>
       <c r="H3" s="11"/>
+      <c r="I3" s="11"/>
+      <c r="J3" s="11"/>
+      <c r="K3" s="11"/>
+      <c r="L3" s="11"/>
+      <c r="M3" s="11"/>
     </row>
     <row r="4" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="10"/>
@@ -6110,11 +6332,16 @@
       <c r="C4" s="10" t="s">
         <v>2</v>
       </c>
-      <c r="D4" s="11"/>
+      <c r="D4" s="10"/>
       <c r="E4" s="11"/>
       <c r="F4" s="11"/>
       <c r="G4" s="11"/>
       <c r="H4" s="11"/>
+      <c r="I4" s="11"/>
+      <c r="J4" s="11"/>
+      <c r="K4" s="11"/>
+      <c r="L4" s="11"/>
+      <c r="M4" s="11"/>
     </row>
     <row r="5" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="10"/>
@@ -6122,21 +6349,31 @@
       <c r="C5" s="10" t="s">
         <v>3</v>
       </c>
-      <c r="D5" s="12"/>
-      <c r="E5" s="11"/>
-      <c r="F5" s="11"/>
-      <c r="G5" s="11"/>
-      <c r="H5" s="11"/>
+      <c r="D5" s="10"/>
+      <c r="E5" s="12"/>
+      <c r="F5" s="12"/>
+      <c r="G5" s="12"/>
+      <c r="H5" s="12"/>
+      <c r="I5" s="12"/>
+      <c r="J5" s="11"/>
+      <c r="K5" s="11"/>
+      <c r="L5" s="11"/>
+      <c r="M5" s="11"/>
     </row>
     <row r="6" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="13"/>
       <c r="B6" s="13"/>
       <c r="C6" s="1"/>
-      <c r="D6" s="7"/>
+      <c r="D6" s="1"/>
       <c r="E6" s="7"/>
       <c r="F6" s="7"/>
       <c r="G6" s="7"/>
       <c r="H6" s="7"/>
+      <c r="I6" s="7"/>
+      <c r="J6" s="7"/>
+      <c r="K6" s="7"/>
+      <c r="L6" s="7"/>
+      <c r="M6" s="7"/>
     </row>
     <row r="7" customFormat="false" ht="13.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A7" s="36" t="s">
@@ -6148,14 +6385,19 @@
       <c r="C7" s="37" t="s">
         <v>52</v>
       </c>
-      <c r="D7" s="37" t="s">
+      <c r="D7" s="37"/>
+      <c r="E7" s="37" t="s">
         <v>53</v>
       </c>
-      <c r="E7" s="37"/>
       <c r="F7" s="37"/>
       <c r="G7" s="37"/>
       <c r="H7" s="37"/>
-      <c r="I7" s="79"/>
+      <c r="I7" s="37"/>
+      <c r="J7" s="37"/>
+      <c r="K7" s="37"/>
+      <c r="L7" s="37"/>
+      <c r="M7" s="37"/>
+      <c r="N7" s="81"/>
     </row>
     <row r="8" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="36"/>
@@ -6163,20 +6405,35 @@
       <c r="C8" s="39" t="s">
         <v>54</v>
       </c>
-      <c r="D8" s="40" t="s">
-        <v>55</v>
+      <c r="D8" s="39" t="s">
+        <v>10</v>
       </c>
       <c r="E8" s="40" t="s">
-        <v>88</v>
+        <v>96</v>
       </c>
       <c r="F8" s="40" t="s">
-        <v>89</v>
+        <v>97</v>
       </c>
       <c r="G8" s="40" t="s">
-        <v>90</v>
+        <v>98</v>
       </c>
       <c r="H8" s="40" t="s">
-        <v>91</v>
+        <v>99</v>
+      </c>
+      <c r="I8" s="40" t="s">
+        <v>100</v>
+      </c>
+      <c r="J8" s="40" t="s">
+        <v>101</v>
+      </c>
+      <c r="K8" s="40" t="s">
+        <v>102</v>
+      </c>
+      <c r="L8" s="40" t="s">
+        <v>103</v>
+      </c>
+      <c r="M8" s="40" t="s">
+        <v>104</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -6185,24 +6442,43 @@
       <c r="C9" s="39" t="s">
         <v>58</v>
       </c>
-      <c r="D9" s="41" t="e">
-        <f aca="false">SUM(D11:D14,#REF!)</f>
-        <v>#REF!</v>
+      <c r="D9" s="39" t="n">
+        <v>63</v>
       </c>
       <c r="E9" s="41" t="n">
-        <f aca="false">SUM(E11:E14)</f>
-        <v>0</v>
+        <f aca="false">D9-7</f>
+        <v>56</v>
       </c>
       <c r="F9" s="41" t="n">
-        <f aca="false">SUM(F11:F14)</f>
-        <v>0</v>
+        <f aca="false">E9-7</f>
+        <v>49</v>
       </c>
       <c r="G9" s="41" t="n">
-        <f aca="false">SUM(G11:G14)</f>
-        <v>0</v>
+        <f aca="false">F9-7</f>
+        <v>42</v>
       </c>
       <c r="H9" s="41" t="n">
-        <f aca="false">SUM(H11:H14)</f>
+        <f aca="false">G9-7</f>
+        <v>35</v>
+      </c>
+      <c r="I9" s="41" t="n">
+        <f aca="false">H9-7</f>
+        <v>28</v>
+      </c>
+      <c r="J9" s="41" t="n">
+        <f aca="false">I9-7</f>
+        <v>21</v>
+      </c>
+      <c r="K9" s="41" t="n">
+        <f aca="false">J9-7</f>
+        <v>14</v>
+      </c>
+      <c r="L9" s="41" t="n">
+        <f aca="false">K9-7</f>
+        <v>7</v>
+      </c>
+      <c r="M9" s="41" t="n">
+        <f aca="false">L9-7</f>
         <v>0</v>
       </c>
     </row>
@@ -6212,289 +6488,329 @@
       <c r="C10" s="39" t="s">
         <v>59</v>
       </c>
-      <c r="D10" s="41"/>
-      <c r="E10" s="41"/>
-      <c r="F10" s="41"/>
-      <c r="G10" s="41"/>
-      <c r="H10" s="41" t="e">
-        <f aca="false">SUM(#REF!)</f>
-        <v>#REF!</v>
+      <c r="D10" s="39" t="n">
+        <f aca="false">SUM(D11:D19)</f>
+        <v>38</v>
+      </c>
+      <c r="E10" s="39" t="n">
+        <f aca="false">SUM(E11:E19)</f>
+        <v>31</v>
+      </c>
+      <c r="F10" s="39" t="n">
+        <f aca="false">SUM(F11:F19)</f>
+        <v>0</v>
+      </c>
+      <c r="G10" s="39" t="n">
+        <f aca="false">SUM(G11:G19)</f>
+        <v>0</v>
+      </c>
+      <c r="H10" s="39" t="n">
+        <f aca="false">SUM(H11:H19)</f>
+        <v>0</v>
+      </c>
+      <c r="I10" s="39" t="n">
+        <f aca="false">SUM(I11:I19)</f>
+        <v>0</v>
+      </c>
+      <c r="J10" s="39" t="n">
+        <f aca="false">SUM(J11:J19)</f>
+        <v>0</v>
+      </c>
+      <c r="K10" s="39" t="n">
+        <f aca="false">SUM(K11:K19)</f>
+        <v>0</v>
+      </c>
+      <c r="L10" s="39" t="n">
+        <f aca="false">SUM(L11:L19)</f>
+        <v>0</v>
+      </c>
+      <c r="M10" s="39" t="n">
+        <f aca="false">SUM(M11:M19)</f>
+        <v>0</v>
       </c>
     </row>
     <row r="11" s="1" customFormat="true" ht="27.65" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A11" s="42" t="s">
-        <v>79</v>
-      </c>
-      <c r="B11" s="85" t="s">
-        <v>93</v>
-      </c>
-      <c r="C11" s="44" t="s">
+        <v>80</v>
+      </c>
+      <c r="B11" s="87" t="s">
+        <v>105</v>
+      </c>
+      <c r="C11" s="61" t="s">
         <v>64</v>
       </c>
-      <c r="D11" s="45" t="n">
+      <c r="D11" s="51" t="n">
         <v>6</v>
       </c>
-      <c r="E11" s="45"/>
-      <c r="F11" s="45"/>
-      <c r="G11" s="45"/>
-      <c r="H11" s="45"/>
-      <c r="AMF11" s="0"/>
-      <c r="AMG11" s="0"/>
-      <c r="AMH11" s="0"/>
-      <c r="AMI11" s="0"/>
-      <c r="AMJ11" s="0"/>
+      <c r="E11" s="51" t="n">
+        <v>5</v>
+      </c>
+      <c r="F11" s="51"/>
+      <c r="G11" s="51"/>
+      <c r="H11" s="51"/>
+      <c r="I11" s="51"/>
+      <c r="J11" s="51"/>
+      <c r="K11" s="51"/>
+      <c r="L11" s="51"/>
+      <c r="M11" s="51"/>
     </row>
     <row r="12" s="1" customFormat="true" ht="27.65" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A12" s="42" t="s">
-        <v>79</v>
-      </c>
-      <c r="B12" s="85" t="s">
-        <v>72</v>
-      </c>
-      <c r="C12" s="44" t="s">
-        <v>81</v>
-      </c>
-      <c r="D12" s="45" t="n">
+        <v>80</v>
+      </c>
+      <c r="B12" s="87" t="s">
+        <v>73</v>
+      </c>
+      <c r="C12" s="61" t="s">
+        <v>82</v>
+      </c>
+      <c r="D12" s="51" t="n">
         <v>4</v>
       </c>
-      <c r="E12" s="45"/>
-      <c r="F12" s="45"/>
-      <c r="G12" s="45"/>
-      <c r="H12" s="45"/>
-      <c r="AMF12" s="0"/>
-      <c r="AMG12" s="0"/>
-      <c r="AMH12" s="0"/>
-      <c r="AMI12" s="0"/>
-      <c r="AMJ12" s="0"/>
+      <c r="E12" s="51" t="n">
+        <v>0</v>
+      </c>
+      <c r="F12" s="51"/>
+      <c r="G12" s="51"/>
+      <c r="H12" s="51"/>
+      <c r="I12" s="51"/>
+      <c r="J12" s="51"/>
+      <c r="K12" s="51"/>
+      <c r="L12" s="51"/>
+      <c r="M12" s="51"/>
     </row>
     <row r="13" s="1" customFormat="true" ht="27.65" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A13" s="42"/>
       <c r="B13" s="42"/>
-      <c r="C13" s="44" t="s">
+      <c r="C13" s="61" t="s">
         <v>66</v>
       </c>
-      <c r="D13" s="45" t="n">
+      <c r="D13" s="51" t="n">
         <v>4</v>
       </c>
-      <c r="E13" s="45"/>
-      <c r="F13" s="45"/>
-      <c r="G13" s="45"/>
-      <c r="H13" s="45"/>
-      <c r="AMF13" s="0"/>
-      <c r="AMG13" s="0"/>
-      <c r="AMH13" s="0"/>
-      <c r="AMI13" s="0"/>
-      <c r="AMJ13" s="0"/>
+      <c r="E13" s="51" t="n">
+        <v>2</v>
+      </c>
+      <c r="F13" s="51"/>
+      <c r="G13" s="51"/>
+      <c r="H13" s="51"/>
+      <c r="I13" s="51"/>
+      <c r="J13" s="51"/>
+      <c r="K13" s="51"/>
+      <c r="L13" s="51"/>
+      <c r="M13" s="51"/>
     </row>
     <row r="14" s="1" customFormat="true" ht="27.65" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A14" s="42"/>
       <c r="B14" s="42"/>
-      <c r="C14" s="44" t="s">
+      <c r="C14" s="61" t="s">
         <v>67</v>
       </c>
-      <c r="D14" s="45" t="n">
+      <c r="D14" s="51" t="n">
         <v>8</v>
       </c>
-      <c r="E14" s="45"/>
-      <c r="F14" s="45"/>
-      <c r="G14" s="45"/>
-      <c r="H14" s="45"/>
-      <c r="AMF14" s="0"/>
-      <c r="AMG14" s="0"/>
-      <c r="AMH14" s="0"/>
-      <c r="AMI14" s="0"/>
-      <c r="AMJ14" s="0"/>
+      <c r="E14" s="51" t="n">
+        <v>8</v>
+      </c>
+      <c r="F14" s="51"/>
+      <c r="G14" s="51"/>
+      <c r="H14" s="51"/>
+      <c r="I14" s="51"/>
+      <c r="J14" s="51"/>
+      <c r="K14" s="51"/>
+      <c r="L14" s="51"/>
+      <c r="M14" s="51"/>
     </row>
     <row r="15" s="1" customFormat="true" ht="27.65" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A15" s="42" t="s">
-        <v>71</v>
-      </c>
-      <c r="B15" s="85" t="s">
         <v>72</v>
       </c>
-      <c r="C15" s="51" t="s">
-        <v>82</v>
-      </c>
-      <c r="D15" s="45" t="n">
+      <c r="B15" s="87" t="s">
+        <v>73</v>
+      </c>
+      <c r="C15" s="62" t="s">
+        <v>95</v>
+      </c>
+      <c r="D15" s="51" t="n">
         <v>8</v>
       </c>
-      <c r="E15" s="45"/>
-      <c r="F15" s="45"/>
-      <c r="G15" s="45"/>
-      <c r="H15" s="45"/>
-      <c r="AMF15" s="0"/>
-      <c r="AMG15" s="0"/>
-      <c r="AMH15" s="0"/>
-      <c r="AMI15" s="0"/>
-      <c r="AMJ15" s="0"/>
+      <c r="E15" s="51" t="n">
+        <v>8</v>
+      </c>
+      <c r="F15" s="51"/>
+      <c r="G15" s="51"/>
+      <c r="H15" s="51"/>
+      <c r="I15" s="51"/>
+      <c r="J15" s="51"/>
+      <c r="K15" s="51"/>
+      <c r="L15" s="51"/>
+      <c r="M15" s="51"/>
     </row>
     <row r="16" s="1" customFormat="true" ht="27.65" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A16" s="42"/>
       <c r="B16" s="42"/>
-      <c r="C16" s="44" t="s">
-        <v>68</v>
-      </c>
-      <c r="D16" s="45" t="n">
+      <c r="C16" s="61" t="s">
+        <v>69</v>
+      </c>
+      <c r="D16" s="51" t="n">
         <v>4</v>
       </c>
-      <c r="E16" s="45"/>
-      <c r="F16" s="45"/>
-      <c r="G16" s="45"/>
-      <c r="H16" s="45"/>
-      <c r="AMF16" s="0"/>
-      <c r="AMG16" s="0"/>
-      <c r="AMH16" s="0"/>
-      <c r="AMI16" s="0"/>
-      <c r="AMJ16" s="0"/>
+      <c r="E16" s="51" t="n">
+        <v>4</v>
+      </c>
+      <c r="F16" s="51"/>
+      <c r="G16" s="51"/>
+      <c r="H16" s="51"/>
+      <c r="I16" s="51"/>
+      <c r="J16" s="51"/>
+      <c r="K16" s="51"/>
+      <c r="L16" s="51"/>
+      <c r="M16" s="51"/>
     </row>
     <row r="17" s="1" customFormat="true" ht="27.65" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A17" s="42"/>
       <c r="B17" s="42"/>
-      <c r="C17" s="50" t="s">
-        <v>83</v>
-      </c>
-      <c r="D17" s="45" t="n">
+      <c r="C17" s="63" t="s">
+        <v>84</v>
+      </c>
+      <c r="D17" s="51" t="n">
         <v>1</v>
       </c>
-      <c r="E17" s="45"/>
-      <c r="F17" s="45"/>
-      <c r="G17" s="45"/>
-      <c r="H17" s="45"/>
-      <c r="AMF17" s="0"/>
-      <c r="AMG17" s="0"/>
-      <c r="AMH17" s="0"/>
-      <c r="AMI17" s="0"/>
-      <c r="AMJ17" s="0"/>
+      <c r="E17" s="51" t="n">
+        <v>1</v>
+      </c>
+      <c r="F17" s="51"/>
+      <c r="G17" s="51"/>
+      <c r="H17" s="51"/>
+      <c r="I17" s="51"/>
+      <c r="J17" s="51"/>
+      <c r="K17" s="51"/>
+      <c r="L17" s="51"/>
+      <c r="M17" s="51"/>
     </row>
     <row r="18" s="1" customFormat="true" ht="27.65" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A18" s="42"/>
       <c r="B18" s="42"/>
-      <c r="C18" s="51" t="s">
-        <v>84</v>
-      </c>
-      <c r="D18" s="45" t="n">
+      <c r="C18" s="62" t="s">
+        <v>85</v>
+      </c>
+      <c r="D18" s="51" t="n">
         <v>1</v>
       </c>
-      <c r="E18" s="45"/>
-      <c r="F18" s="45"/>
-      <c r="G18" s="45"/>
-      <c r="H18" s="45"/>
-      <c r="AMF18" s="0"/>
-      <c r="AMG18" s="0"/>
-      <c r="AMH18" s="0"/>
-      <c r="AMI18" s="0"/>
-      <c r="AMJ18" s="0"/>
+      <c r="E18" s="51" t="n">
+        <v>1</v>
+      </c>
+      <c r="F18" s="51"/>
+      <c r="G18" s="51"/>
+      <c r="H18" s="51"/>
+      <c r="I18" s="51"/>
+      <c r="J18" s="51"/>
+      <c r="K18" s="51"/>
+      <c r="L18" s="51"/>
+      <c r="M18" s="51"/>
     </row>
     <row r="19" s="1" customFormat="true" ht="27.65" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A19" s="42"/>
       <c r="B19" s="42"/>
-      <c r="C19" s="50" t="s">
-        <v>85</v>
-      </c>
-      <c r="D19" s="45" t="n">
+      <c r="C19" s="63" t="s">
+        <v>86</v>
+      </c>
+      <c r="D19" s="51" t="n">
         <v>2</v>
       </c>
-      <c r="E19" s="45"/>
-      <c r="F19" s="45"/>
-      <c r="G19" s="45"/>
-      <c r="H19" s="45"/>
-      <c r="AMF19" s="0"/>
-      <c r="AMG19" s="0"/>
-      <c r="AMH19" s="0"/>
-      <c r="AMI19" s="0"/>
-      <c r="AMJ19" s="0"/>
+      <c r="E19" s="51" t="n">
+        <v>2</v>
+      </c>
+      <c r="F19" s="51"/>
+      <c r="G19" s="51"/>
+      <c r="H19" s="51"/>
+      <c r="I19" s="51"/>
+      <c r="J19" s="51"/>
+      <c r="K19" s="51"/>
+      <c r="L19" s="51"/>
+      <c r="M19" s="51"/>
     </row>
     <row r="20" s="1" customFormat="true" ht="27.65" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A20" s="42"/>
       <c r="B20" s="42"/>
       <c r="C20" s="52" t="s">
-        <v>76</v>
-      </c>
-      <c r="D20" s="53" t="n">
+        <v>77</v>
+      </c>
+      <c r="D20" s="48" t="n">
         <v>1</v>
       </c>
-      <c r="E20" s="45"/>
-      <c r="F20" s="45"/>
-      <c r="G20" s="45"/>
-      <c r="H20" s="45"/>
-      <c r="AMF20" s="0"/>
-      <c r="AMG20" s="0"/>
-      <c r="AMH20" s="0"/>
-      <c r="AMI20" s="0"/>
-      <c r="AMJ20" s="0"/>
+      <c r="E20" s="48" t="n">
+        <v>1</v>
+      </c>
+      <c r="F20" s="48"/>
+      <c r="G20" s="48"/>
+      <c r="H20" s="48"/>
+      <c r="I20" s="48"/>
+      <c r="J20" s="51"/>
+      <c r="K20" s="51"/>
+      <c r="L20" s="51"/>
+      <c r="M20" s="51"/>
     </row>
     <row r="21" s="1" customFormat="true" ht="34.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A21" s="42"/>
-      <c r="B21" s="54" t="s">
-        <v>77</v>
-      </c>
-      <c r="C21" s="54"/>
-      <c r="D21" s="54"/>
-      <c r="E21" s="54"/>
-      <c r="F21" s="54"/>
-      <c r="G21" s="54"/>
-      <c r="H21" s="54"/>
-      <c r="AMF21" s="0"/>
-      <c r="AMG21" s="0"/>
-      <c r="AMH21" s="0"/>
-      <c r="AMI21" s="0"/>
-      <c r="AMJ21" s="0"/>
+      <c r="B21" s="53" t="s">
+        <v>78</v>
+      </c>
+      <c r="C21" s="53"/>
+      <c r="D21" s="53"/>
+      <c r="E21" s="53"/>
+      <c r="F21" s="53"/>
+      <c r="G21" s="53"/>
+      <c r="H21" s="53"/>
+      <c r="I21" s="53"/>
+      <c r="J21" s="53"/>
+      <c r="K21" s="53"/>
+      <c r="L21" s="53"/>
+      <c r="M21" s="53"/>
     </row>
     <row r="22" s="1" customFormat="true" ht="34.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A22" s="42"/>
-      <c r="B22" s="55" t="s">
-        <v>78</v>
-      </c>
-      <c r="C22" s="56" t="n">
-        <f aca="false">SUM(D11:D21)</f>
-        <v>39</v>
+      <c r="B22" s="54" t="s">
+        <v>79</v>
+      </c>
+      <c r="C22" s="55" t="n">
+        <f aca="false">SUM(E11:E21)</f>
+        <v>32</v>
       </c>
       <c r="D22" s="55"/>
-      <c r="E22" s="55"/>
-      <c r="F22" s="55"/>
-      <c r="G22" s="55"/>
-      <c r="H22" s="55"/>
-      <c r="I22" s="48"/>
-      <c r="J22" s="48"/>
-      <c r="AMF22" s="0"/>
-      <c r="AMG22" s="0"/>
-      <c r="AMH22" s="0"/>
-      <c r="AMI22" s="0"/>
-      <c r="AMJ22" s="0"/>
+      <c r="E22" s="54"/>
+      <c r="F22" s="54"/>
+      <c r="G22" s="54"/>
+      <c r="H22" s="54"/>
+      <c r="I22" s="54"/>
+      <c r="J22" s="54"/>
+      <c r="K22" s="54"/>
+      <c r="L22" s="54"/>
+      <c r="M22" s="54"/>
+      <c r="N22" s="46"/>
+      <c r="O22" s="46"/>
     </row>
     <row r="23" s="1" customFormat="true" ht="8.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A23" s="64"/>
-      <c r="B23" s="65"/>
-      <c r="C23" s="66"/>
-      <c r="D23" s="67"/>
-      <c r="E23" s="67"/>
-      <c r="F23" s="67"/>
-      <c r="G23" s="67"/>
-      <c r="H23" s="68"/>
-      <c r="AMF23" s="0"/>
-      <c r="AMG23" s="0"/>
-      <c r="AMH23" s="0"/>
-      <c r="AMI23" s="0"/>
-      <c r="AMJ23" s="0"/>
-    </row>
-    <row r="1048565" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048566" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048567" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048568" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048569" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048570" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048571" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048572" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048573" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048574" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048575" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048576" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+      <c r="A23" s="66"/>
+      <c r="B23" s="67"/>
+      <c r="C23" s="68"/>
+      <c r="D23" s="68"/>
+      <c r="E23" s="69"/>
+      <c r="F23" s="69"/>
+      <c r="G23" s="69"/>
+      <c r="H23" s="69"/>
+      <c r="I23" s="69"/>
+      <c r="J23" s="69"/>
+      <c r="K23" s="69"/>
+      <c r="L23" s="69"/>
+      <c r="M23" s="70"/>
+    </row>
   </sheetData>
   <mergeCells count="6">
-    <mergeCell ref="A2:H2"/>
+    <mergeCell ref="A2:M2"/>
     <mergeCell ref="A7:A10"/>
     <mergeCell ref="B7:B10"/>
-    <mergeCell ref="D7:H7"/>
+    <mergeCell ref="E7:M7"/>
     <mergeCell ref="A11:A22"/>
     <mergeCell ref="B11:B20"/>
   </mergeCells>
@@ -6615,7 +6931,7 @@
       <c r="F7" s="37"/>
       <c r="G7" s="37"/>
       <c r="H7" s="37"/>
-      <c r="I7" s="79"/>
+      <c r="I7" s="81"/>
     </row>
     <row r="8" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="36"/>
@@ -6627,16 +6943,16 @@
         <v>55</v>
       </c>
       <c r="E8" s="40" t="s">
-        <v>88</v>
+        <v>90</v>
       </c>
       <c r="F8" s="40" t="s">
-        <v>89</v>
+        <v>91</v>
       </c>
       <c r="G8" s="40" t="s">
-        <v>90</v>
+        <v>92</v>
       </c>
       <c r="H8" s="40" t="s">
-        <v>91</v>
+        <v>93</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -6683,21 +6999,21 @@
     </row>
     <row r="11" s="1" customFormat="true" ht="27.65" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A11" s="42" t="s">
-        <v>79</v>
-      </c>
-      <c r="B11" s="85" t="s">
-        <v>94</v>
-      </c>
-      <c r="C11" s="44" t="s">
+        <v>80</v>
+      </c>
+      <c r="B11" s="87" t="s">
+        <v>106</v>
+      </c>
+      <c r="C11" s="61" t="s">
         <v>64</v>
       </c>
-      <c r="D11" s="45" t="n">
+      <c r="D11" s="51" t="n">
         <v>6</v>
       </c>
-      <c r="E11" s="45"/>
-      <c r="F11" s="45"/>
-      <c r="G11" s="45"/>
-      <c r="H11" s="45"/>
+      <c r="E11" s="51"/>
+      <c r="F11" s="51"/>
+      <c r="G11" s="51"/>
+      <c r="H11" s="51"/>
       <c r="AMF11" s="0"/>
       <c r="AMG11" s="0"/>
       <c r="AMH11" s="0"/>
@@ -6706,21 +7022,21 @@
     </row>
     <row r="12" s="1" customFormat="true" ht="27.65" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A12" s="42" t="s">
-        <v>79</v>
-      </c>
-      <c r="B12" s="85" t="s">
-        <v>72</v>
-      </c>
-      <c r="C12" s="44" t="s">
-        <v>81</v>
-      </c>
-      <c r="D12" s="45" t="n">
+        <v>80</v>
+      </c>
+      <c r="B12" s="87" t="s">
+        <v>73</v>
+      </c>
+      <c r="C12" s="61" t="s">
+        <v>82</v>
+      </c>
+      <c r="D12" s="51" t="n">
         <v>4</v>
       </c>
-      <c r="E12" s="45"/>
-      <c r="F12" s="45"/>
-      <c r="G12" s="45"/>
-      <c r="H12" s="45"/>
+      <c r="E12" s="51"/>
+      <c r="F12" s="51"/>
+      <c r="G12" s="51"/>
+      <c r="H12" s="51"/>
       <c r="AMF12" s="0"/>
       <c r="AMG12" s="0"/>
       <c r="AMH12" s="0"/>
@@ -6730,16 +7046,16 @@
     <row r="13" s="1" customFormat="true" ht="27.65" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A13" s="42"/>
       <c r="B13" s="42"/>
-      <c r="C13" s="44" t="s">
+      <c r="C13" s="61" t="s">
         <v>66</v>
       </c>
-      <c r="D13" s="45" t="n">
+      <c r="D13" s="51" t="n">
         <v>4</v>
       </c>
-      <c r="E13" s="45"/>
-      <c r="F13" s="45"/>
-      <c r="G13" s="45"/>
-      <c r="H13" s="45"/>
+      <c r="E13" s="51"/>
+      <c r="F13" s="51"/>
+      <c r="G13" s="51"/>
+      <c r="H13" s="51"/>
       <c r="AMF13" s="0"/>
       <c r="AMG13" s="0"/>
       <c r="AMH13" s="0"/>
@@ -6749,16 +7065,16 @@
     <row r="14" s="1" customFormat="true" ht="27.65" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A14" s="42"/>
       <c r="B14" s="42"/>
-      <c r="C14" s="44" t="s">
+      <c r="C14" s="61" t="s">
         <v>67</v>
       </c>
-      <c r="D14" s="45" t="n">
+      <c r="D14" s="51" t="n">
         <v>8</v>
       </c>
-      <c r="E14" s="45"/>
-      <c r="F14" s="45"/>
-      <c r="G14" s="45"/>
-      <c r="H14" s="45"/>
+      <c r="E14" s="51"/>
+      <c r="F14" s="51"/>
+      <c r="G14" s="51"/>
+      <c r="H14" s="51"/>
       <c r="AMF14" s="0"/>
       <c r="AMG14" s="0"/>
       <c r="AMH14" s="0"/>
@@ -6767,21 +7083,21 @@
     </row>
     <row r="15" s="1" customFormat="true" ht="27.65" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A15" s="42" t="s">
-        <v>71</v>
-      </c>
-      <c r="B15" s="85" t="s">
         <v>72</v>
       </c>
-      <c r="C15" s="51" t="s">
-        <v>82</v>
-      </c>
-      <c r="D15" s="45" t="n">
+      <c r="B15" s="87" t="s">
+        <v>73</v>
+      </c>
+      <c r="C15" s="62" t="s">
+        <v>95</v>
+      </c>
+      <c r="D15" s="51" t="n">
         <v>8</v>
       </c>
-      <c r="E15" s="45"/>
-      <c r="F15" s="45"/>
-      <c r="G15" s="45"/>
-      <c r="H15" s="45"/>
+      <c r="E15" s="51"/>
+      <c r="F15" s="51"/>
+      <c r="G15" s="51"/>
+      <c r="H15" s="51"/>
       <c r="AMF15" s="0"/>
       <c r="AMG15" s="0"/>
       <c r="AMH15" s="0"/>
@@ -6791,16 +7107,16 @@
     <row r="16" s="1" customFormat="true" ht="27.65" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A16" s="42"/>
       <c r="B16" s="42"/>
-      <c r="C16" s="44" t="s">
-        <v>68</v>
-      </c>
-      <c r="D16" s="45" t="n">
+      <c r="C16" s="61" t="s">
+        <v>69</v>
+      </c>
+      <c r="D16" s="51" t="n">
         <v>4</v>
       </c>
-      <c r="E16" s="45"/>
-      <c r="F16" s="45"/>
-      <c r="G16" s="45"/>
-      <c r="H16" s="45"/>
+      <c r="E16" s="51"/>
+      <c r="F16" s="51"/>
+      <c r="G16" s="51"/>
+      <c r="H16" s="51"/>
       <c r="AMF16" s="0"/>
       <c r="AMG16" s="0"/>
       <c r="AMH16" s="0"/>
@@ -6810,16 +7126,16 @@
     <row r="17" s="1" customFormat="true" ht="27.65" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A17" s="42"/>
       <c r="B17" s="42"/>
-      <c r="C17" s="50" t="s">
-        <v>83</v>
-      </c>
-      <c r="D17" s="45" t="n">
+      <c r="C17" s="63" t="s">
+        <v>84</v>
+      </c>
+      <c r="D17" s="51" t="n">
         <v>1</v>
       </c>
-      <c r="E17" s="45"/>
-      <c r="F17" s="45"/>
-      <c r="G17" s="45"/>
-      <c r="H17" s="45"/>
+      <c r="E17" s="51"/>
+      <c r="F17" s="51"/>
+      <c r="G17" s="51"/>
+      <c r="H17" s="51"/>
       <c r="AMF17" s="0"/>
       <c r="AMG17" s="0"/>
       <c r="AMH17" s="0"/>
@@ -6829,16 +7145,16 @@
     <row r="18" s="1" customFormat="true" ht="27.65" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A18" s="42"/>
       <c r="B18" s="42"/>
-      <c r="C18" s="51" t="s">
-        <v>84</v>
-      </c>
-      <c r="D18" s="45" t="n">
+      <c r="C18" s="62" t="s">
+        <v>85</v>
+      </c>
+      <c r="D18" s="51" t="n">
         <v>1</v>
       </c>
-      <c r="E18" s="45"/>
-      <c r="F18" s="45"/>
-      <c r="G18" s="45"/>
-      <c r="H18" s="45"/>
+      <c r="E18" s="51"/>
+      <c r="F18" s="51"/>
+      <c r="G18" s="51"/>
+      <c r="H18" s="51"/>
       <c r="AMF18" s="0"/>
       <c r="AMG18" s="0"/>
       <c r="AMH18" s="0"/>
@@ -6848,16 +7164,16 @@
     <row r="19" s="1" customFormat="true" ht="27.65" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A19" s="42"/>
       <c r="B19" s="42"/>
-      <c r="C19" s="50" t="s">
-        <v>85</v>
-      </c>
-      <c r="D19" s="45" t="n">
+      <c r="C19" s="63" t="s">
+        <v>86</v>
+      </c>
+      <c r="D19" s="51" t="n">
         <v>2</v>
       </c>
-      <c r="E19" s="45"/>
-      <c r="F19" s="45"/>
-      <c r="G19" s="45"/>
-      <c r="H19" s="45"/>
+      <c r="E19" s="51"/>
+      <c r="F19" s="51"/>
+      <c r="G19" s="51"/>
+      <c r="H19" s="51"/>
       <c r="AMF19" s="0"/>
       <c r="AMG19" s="0"/>
       <c r="AMH19" s="0"/>
@@ -6868,15 +7184,15 @@
       <c r="A20" s="42"/>
       <c r="B20" s="42"/>
       <c r="C20" s="52" t="s">
-        <v>76</v>
-      </c>
-      <c r="D20" s="53" t="n">
+        <v>77</v>
+      </c>
+      <c r="D20" s="48" t="n">
         <v>1</v>
       </c>
-      <c r="E20" s="45"/>
-      <c r="F20" s="45"/>
-      <c r="G20" s="45"/>
-      <c r="H20" s="45"/>
+      <c r="E20" s="51"/>
+      <c r="F20" s="51"/>
+      <c r="G20" s="51"/>
+      <c r="H20" s="51"/>
       <c r="AMF20" s="0"/>
       <c r="AMG20" s="0"/>
       <c r="AMH20" s="0"/>
@@ -6885,15 +7201,15 @@
     </row>
     <row r="21" s="1" customFormat="true" ht="34.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A21" s="42"/>
-      <c r="B21" s="54" t="s">
-        <v>77</v>
-      </c>
-      <c r="C21" s="54"/>
-      <c r="D21" s="54"/>
-      <c r="E21" s="54"/>
-      <c r="F21" s="54"/>
-      <c r="G21" s="54"/>
-      <c r="H21" s="54"/>
+      <c r="B21" s="53" t="s">
+        <v>78</v>
+      </c>
+      <c r="C21" s="53"/>
+      <c r="D21" s="53"/>
+      <c r="E21" s="53"/>
+      <c r="F21" s="53"/>
+      <c r="G21" s="53"/>
+      <c r="H21" s="53"/>
       <c r="AMF21" s="0"/>
       <c r="AMG21" s="0"/>
       <c r="AMH21" s="0"/>
@@ -6902,20 +7218,20 @@
     </row>
     <row r="22" s="1" customFormat="true" ht="34.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A22" s="42"/>
-      <c r="B22" s="55" t="s">
-        <v>78</v>
-      </c>
-      <c r="C22" s="56" t="n">
+      <c r="B22" s="54" t="s">
+        <v>79</v>
+      </c>
+      <c r="C22" s="55" t="n">
         <f aca="false">SUM(D11:D21)</f>
         <v>39</v>
       </c>
-      <c r="D22" s="55"/>
-      <c r="E22" s="55"/>
-      <c r="F22" s="55"/>
-      <c r="G22" s="55"/>
-      <c r="H22" s="55"/>
-      <c r="I22" s="48"/>
-      <c r="J22" s="48"/>
+      <c r="D22" s="54"/>
+      <c r="E22" s="54"/>
+      <c r="F22" s="54"/>
+      <c r="G22" s="54"/>
+      <c r="H22" s="54"/>
+      <c r="I22" s="46"/>
+      <c r="J22" s="46"/>
       <c r="AMF22" s="0"/>
       <c r="AMG22" s="0"/>
       <c r="AMH22" s="0"/>
@@ -6923,14 +7239,14 @@
       <c r="AMJ22" s="0"/>
     </row>
     <row r="23" s="1" customFormat="true" ht="8.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A23" s="64"/>
-      <c r="B23" s="65"/>
-      <c r="C23" s="66"/>
-      <c r="D23" s="67"/>
-      <c r="E23" s="67"/>
-      <c r="F23" s="67"/>
-      <c r="G23" s="67"/>
-      <c r="H23" s="68"/>
+      <c r="A23" s="66"/>
+      <c r="B23" s="67"/>
+      <c r="C23" s="68"/>
+      <c r="D23" s="69"/>
+      <c r="E23" s="69"/>
+      <c r="F23" s="69"/>
+      <c r="G23" s="69"/>
+      <c r="H23" s="70"/>
       <c r="AMF23" s="0"/>
       <c r="AMG23" s="0"/>
       <c r="AMH23" s="0"/>

</xml_diff>